<commit_message>
sistemazione codice e file excel, nel codice ho messo i valori in Volt e Amper, così da trovare una relazione corretta. I dati vengono. Il coeff. delle rette è da aggisutare rispetto a "e" e agli altri parametri.
</commit_message>
<xml_diff>
--- a/relazioni/esperienza_2/codici/Esperienza_2.xlsx
+++ b/relazioni/esperienza_2/codici/Esperienza_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alessiobrusini/Desktop/LABORATORIO-DI-ELETTROMAGNETISMO/relazioni/esperienza_2/codici/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73688E18-612B-8A49-ABAF-B2FA67B07B53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A1CEFA6-7174-B641-BFF8-20D50D56E44E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="27100" windowHeight="15920" activeTab="4" xr2:uid="{9832D23C-5E2D-EB46-85A1-EE46353BB05C}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="27100" windowHeight="15920" activeTab="5" xr2:uid="{9832D23C-5E2D-EB46-85A1-EE46353BB05C}"/>
   </bookViews>
   <sheets>
     <sheet name="Temp_1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="23">
   <si>
     <t>n.</t>
   </si>
@@ -85,9 +85,6 @@
       </rPr>
       <t>R_din(Ω)</t>
     </r>
-  </si>
-  <si>
-    <t>lnCorr(mA)</t>
   </si>
   <si>
     <t>Colonna2</t>
@@ -317,7 +314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -342,7 +339,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1245,7 +1241,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>lnCorr(mA)</c:v>
+                  <c:v>lnCorr(A)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4684,7 +4680,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>lnCorr(mA)</c:v>
+                  <c:v>lnCorr(A)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -11294,7 +11290,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>lnCorr(mA)</c:v>
+                  <c:v>lnCorr(A)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -32226,10 +32222,10 @@
         <v>9</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AC1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -32819,7 +32815,7 @@
         <v>21.874922762723592</v>
       </c>
       <c r="J16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M16">
         <f t="shared" si="2"/>
@@ -32946,7 +32942,7 @@
         <v>21.776961407646436</v>
       </c>
       <c r="J19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M19">
         <f t="shared" si="2"/>
@@ -33074,7 +33070,7 @@
         <v>21.713794811313498</v>
       </c>
       <c r="J22" s="14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M22">
         <f t="shared" si="2"/>
@@ -33117,7 +33113,7 @@
         <v>21.720318408973505</v>
       </c>
       <c r="J23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M23">
         <f t="shared" si="2"/>
@@ -34528,7 +34524,7 @@
     </row>
     <row r="60" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B60" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C60" s="18"/>
       <c r="D60" s="18"/>
@@ -34573,8 +34569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E64FDFDC-13B1-AB4C-B1C3-7FF9E2CAD166}">
   <dimension ref="A1:AC35"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="75" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="X65" sqref="X65"/>
+    <sheetView topLeftCell="H1" zoomScale="75" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -34617,10 +34613,10 @@
         <v>9</v>
       </c>
       <c r="AB1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC1" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="AC1" s="4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -35210,7 +35206,7 @@
         <v>22.415946180830719</v>
       </c>
       <c r="J16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M16">
         <f t="shared" si="1"/>
@@ -35337,7 +35333,7 @@
         <v>21.691682976280454</v>
       </c>
       <c r="J19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M19">
         <f t="shared" si="1"/>
@@ -35465,7 +35461,7 @@
         <v>20.304714979371081</v>
       </c>
       <c r="J22" s="14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M22">
         <f t="shared" si="1"/>
@@ -35508,7 +35504,7 @@
         <v>19.839554416671128</v>
       </c>
       <c r="J23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M23">
         <f t="shared" si="1"/>
@@ -35874,7 +35870,7 @@
     <row r="33" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B34" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C34" s="18"/>
       <c r="D34" s="18"/>
@@ -35906,8 +35902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B8D5F5-4DDF-2344-BE93-713864C91CD6}">
   <dimension ref="A1:AC58"/>
   <sheetViews>
-    <sheetView topLeftCell="J13" zoomScale="70" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="AB9" sqref="AB9"/>
+    <sheetView topLeftCell="J1" zoomScale="70" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -35950,10 +35946,10 @@
         <v>9</v>
       </c>
       <c r="AB1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC1" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="AC1" s="4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -36544,7 +36540,7 @@
         <v>23.781163495180113</v>
       </c>
       <c r="J16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M16">
         <f t="shared" si="2"/>
@@ -36671,7 +36667,7 @@
         <v>22.613512259737554</v>
       </c>
       <c r="J19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M19">
         <f t="shared" si="2"/>
@@ -36799,7 +36795,7 @@
         <v>17.359081700246044</v>
       </c>
       <c r="J22" s="14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M22">
         <f t="shared" si="2"/>
@@ -36842,7 +36838,7 @@
         <v>14.868092397968583</v>
       </c>
       <c r="J23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M23">
         <f t="shared" si="2"/>
@@ -36888,7 +36884,7 @@
     <row r="56" spans="9:14" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="57" spans="9:14" x14ac:dyDescent="0.2">
       <c r="I57" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J57" s="18"/>
       <c r="K57" s="18"/>
@@ -36968,10 +36964,10 @@
         <v>9</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AC1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -37804,7 +37800,7 @@
     <row r="22" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B23" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C23" s="18"/>
       <c r="D23" s="18"/>
@@ -37822,7 +37818,7 @@
     </row>
     <row r="37" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G37" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="7:7" ht="18" x14ac:dyDescent="0.2">
@@ -37833,7 +37829,7 @@
     </row>
     <row r="40" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G40" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="7:7" ht="17" x14ac:dyDescent="0.2">
@@ -37847,12 +37843,12 @@
     </row>
     <row r="43" spans="7:7" ht="20" x14ac:dyDescent="0.2">
       <c r="G43" s="14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G44" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -37869,10 +37865,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29EA75CD-2EAA-AD46-B54B-F32D80398925}">
-  <dimension ref="A1:AC64"/>
+  <dimension ref="A1:AC50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="75" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView topLeftCell="G1" zoomScale="75" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -37912,10 +37908,10 @@
         <v>7</v>
       </c>
       <c r="I1" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="17" t="s">
         <v>19</v>
-      </c>
-      <c r="J1" s="17" t="s">
-        <v>20</v>
       </c>
       <c r="M1" t="s">
         <v>8</v>
@@ -37924,10 +37920,10 @@
         <v>9</v>
       </c>
       <c r="AB1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC1" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="AC1" s="4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -39176,175 +39172,60 @@
         <f t="shared" si="3"/>
         <v>6.6325231377546354E-3</v>
       </c>
-      <c r="AB31" s="20"/>
-      <c r="AC31" s="20"/>
     </row>
-    <row r="32" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AB32" s="20"/>
-      <c r="AC32" s="20"/>
-    </row>
-    <row r="33" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B33" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C33" s="18"/>
       <c r="D33" s="18"/>
       <c r="E33" s="18"/>
       <c r="F33" s="18"/>
       <c r="G33" s="18"/>
-      <c r="AB33" s="20"/>
-      <c r="AC33" s="20"/>
     </row>
-    <row r="34" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B34" s="19"/>
       <c r="C34" s="19"/>
       <c r="D34" s="19"/>
       <c r="E34" s="19"/>
       <c r="F34" s="19"/>
       <c r="G34" s="19"/>
-      <c r="AB34" s="20"/>
-      <c r="AC34" s="20"/>
     </row>
-    <row r="35" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="AB35" s="20"/>
-      <c r="AC35" s="20"/>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="H43" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="36" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="AB36" s="20"/>
-      <c r="AC36" s="20"/>
-    </row>
-    <row r="37" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="AB37" s="20"/>
-      <c r="AC37" s="20"/>
-    </row>
-    <row r="38" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="AB38" s="20"/>
-      <c r="AC38" s="20"/>
-    </row>
-    <row r="39" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="AB39" s="20"/>
-      <c r="AC39" s="20"/>
-    </row>
-    <row r="40" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="AB40" s="20"/>
-      <c r="AC40" s="20"/>
-    </row>
-    <row r="41" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="AB41" s="20"/>
-      <c r="AC41" s="20"/>
-    </row>
-    <row r="42" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="AB42" s="20"/>
-      <c r="AC42" s="20"/>
-    </row>
-    <row r="43" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="H43" t="s">
-        <v>12</v>
-      </c>
-      <c r="AB43" s="20"/>
-      <c r="AC43" s="20"/>
-    </row>
-    <row r="44" spans="2:29" ht="18" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:8" ht="18" x14ac:dyDescent="0.2">
       <c r="H44" s="9">
         <f>1.602176634*10^(-19)</f>
         <v>1.6021766340000001E-19</v>
       </c>
-      <c r="AB44" s="20"/>
-      <c r="AC44" s="20"/>
     </row>
-    <row r="45" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="AB45" s="20"/>
-      <c r="AC45" s="20"/>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="H46" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="46" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="H46" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB46" s="20"/>
-      <c r="AC46" s="20"/>
-    </row>
-    <row r="47" spans="2:29" ht="17" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:8" ht="17" x14ac:dyDescent="0.2">
       <c r="H47" s="11">
         <f>1.3806503*10^(-23)</f>
         <v>1.3806503000000004E-23</v>
       </c>
-      <c r="AB47" s="20"/>
-      <c r="AC47" s="20"/>
     </row>
-    <row r="48" spans="2:29" ht="18" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:8" ht="18" x14ac:dyDescent="0.2">
       <c r="H48" s="10"/>
-      <c r="AB48" s="20"/>
-      <c r="AC48" s="20"/>
     </row>
-    <row r="49" spans="8:29" ht="20" x14ac:dyDescent="0.2">
+    <row r="49" spans="8:8" ht="20" x14ac:dyDescent="0.2">
       <c r="H49" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H50" t="s">
         <v>14</v>
       </c>
-      <c r="AB49" s="20"/>
-      <c r="AC49" s="20"/>
-    </row>
-    <row r="50" spans="8:29" x14ac:dyDescent="0.2">
-      <c r="H50" t="s">
-        <v>15</v>
-      </c>
-      <c r="AB50" s="20"/>
-      <c r="AC50" s="20"/>
-    </row>
-    <row r="51" spans="8:29" x14ac:dyDescent="0.2">
-      <c r="AB51" s="20"/>
-      <c r="AC51" s="20"/>
-    </row>
-    <row r="52" spans="8:29" x14ac:dyDescent="0.2">
-      <c r="AB52" s="20"/>
-      <c r="AC52" s="20"/>
-    </row>
-    <row r="53" spans="8:29" x14ac:dyDescent="0.2">
-      <c r="AB53" s="20"/>
-      <c r="AC53" s="20"/>
-    </row>
-    <row r="54" spans="8:29" x14ac:dyDescent="0.2">
-      <c r="AB54" s="20"/>
-      <c r="AC54" s="20"/>
-    </row>
-    <row r="55" spans="8:29" x14ac:dyDescent="0.2">
-      <c r="AB55" s="20"/>
-      <c r="AC55" s="20"/>
-    </row>
-    <row r="56" spans="8:29" x14ac:dyDescent="0.2">
-      <c r="AB56" s="20"/>
-      <c r="AC56" s="20"/>
-    </row>
-    <row r="57" spans="8:29" x14ac:dyDescent="0.2">
-      <c r="AB57" s="20"/>
-      <c r="AC57" s="20"/>
-    </row>
-    <row r="58" spans="8:29" x14ac:dyDescent="0.2">
-      <c r="AB58" s="20"/>
-      <c r="AC58" s="20"/>
-    </row>
-    <row r="59" spans="8:29" x14ac:dyDescent="0.2">
-      <c r="AB59" s="20"/>
-      <c r="AC59" s="20"/>
-    </row>
-    <row r="60" spans="8:29" x14ac:dyDescent="0.2">
-      <c r="AB60" s="20"/>
-      <c r="AC60" s="20"/>
-    </row>
-    <row r="61" spans="8:29" x14ac:dyDescent="0.2">
-      <c r="AB61" s="20"/>
-      <c r="AC61" s="20"/>
-    </row>
-    <row r="62" spans="8:29" x14ac:dyDescent="0.2">
-      <c r="AB62" s="20"/>
-      <c r="AC62" s="20"/>
-    </row>
-    <row r="63" spans="8:29" x14ac:dyDescent="0.2">
-      <c r="AB63" s="20"/>
-      <c r="AC63" s="20"/>
-    </row>
-    <row r="64" spans="8:29" x14ac:dyDescent="0.2">
-      <c r="AB64" s="20"/>
-      <c r="AC64" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -39360,9 +39241,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{964810A6-0329-CE44-9434-FAE1DDC1CC77}">
-  <dimension ref="A1:AD58"/>
+  <dimension ref="A1:AC58"/>
   <sheetViews>
-    <sheetView topLeftCell="Q31" zoomScale="125" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="61" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -39406,10 +39287,10 @@
         <v>9</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AC1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -39443,7 +39324,7 @@
         <v>1.2499999999999998</v>
       </c>
       <c r="N2">
-        <f t="shared" ref="N2:N23" si="0">M2*(2*E3/(D3-D2)+2*G3/(F3-F2))</f>
+        <f t="shared" ref="N2:N19" si="0">M2*(2*E3/(D3-D2)+2*G3/(F3-F2))</f>
         <v>-0.84374999999999978</v>
       </c>
       <c r="AB2" s="5">
@@ -39479,7 +39360,7 @@
         <v>35.109968964181618</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M23" si="2">(D4-D3)/(F4-F3)</f>
+        <f t="shared" ref="M3:M19" si="2">(D4-D3)/(F4-F3)</f>
         <v>1.4354066985645935</v>
       </c>
       <c r="N3">
@@ -39487,7 +39368,7 @@
         <v>-0.97067374831162301</v>
       </c>
       <c r="AB3" s="5">
-        <f t="shared" ref="AB3:AB20" si="3">LN(F3/1000)</f>
+        <f t="shared" ref="AB3:AB19" si="3">LN(F3/1000)</f>
         <v>-4.4022293419914007</v>
       </c>
       <c r="AC3" s="8"/>
@@ -39999,7 +39880,7 @@
         <v>33.718819250506492</v>
       </c>
       <c r="J16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M16">
         <f t="shared" si="2"/>
@@ -40015,7 +39896,7 @@
       </c>
       <c r="AC16" s="6"/>
     </row>
-    <row r="17" spans="1:30" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" ht="19" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>15</v>
       </c>
@@ -40059,7 +39940,7 @@
       </c>
       <c r="AC17" s="8"/>
     </row>
-    <row r="18" spans="1:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>16</v>
       </c>
@@ -40099,7 +39980,7 @@
       </c>
       <c r="AC18" s="6"/>
     </row>
-    <row r="19" spans="1:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>17</v>
       </c>
@@ -40126,7 +40007,7 @@
         <v>32.327669536831372</v>
       </c>
       <c r="J19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M19">
         <f t="shared" si="2"/>
@@ -40142,7 +40023,7 @@
       </c>
       <c r="AC19" s="8"/>
     </row>
-    <row r="20" spans="1:30" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="5">
         <v>18</v>
       </c>
@@ -40173,100 +40054,23 @@
         <v>1.3806503000000004E-23</v>
       </c>
       <c r="AB20" s="5"/>
-      <c r="AC20" s="20"/>
-      <c r="AD20" s="20"/>
     </row>
-    <row r="21" spans="1:30" ht="18" x14ac:dyDescent="0.2">
-      <c r="A21" s="20"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
+    <row r="21" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="J21" s="10"/>
-      <c r="AB21" s="20"/>
-      <c r="AC21" s="20"/>
-      <c r="AD21" s="20"/>
     </row>
-    <row r="22" spans="1:30" ht="20" x14ac:dyDescent="0.2">
-      <c r="A22" s="20"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
+    <row r="22" spans="1:29" ht="20" x14ac:dyDescent="0.2">
       <c r="J22" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="J23" t="s">
         <v>14</v>
       </c>
-      <c r="AB22" s="20"/>
-      <c r="AC22" s="20"/>
-      <c r="AD22" s="20"/>
-    </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A23" s="20"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" t="s">
-        <v>15</v>
-      </c>
-      <c r="AB23" s="20"/>
-      <c r="AC23" s="20"/>
-      <c r="AD23" s="20"/>
-    </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A24" s="20"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
-      <c r="AB24" s="20"/>
-      <c r="AC24" s="20"/>
-      <c r="AD24" s="20"/>
-    </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A25" s="20"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
-      <c r="AB25" s="20"/>
-      <c r="AC25" s="20"/>
-      <c r="AD25" s="20"/>
-    </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A26" s="20"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
     </row>
     <row r="44" spans="27:27" x14ac:dyDescent="0.2">
       <c r="AA44" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="45" spans="27:27" x14ac:dyDescent="0.2">
@@ -40277,7 +40081,7 @@
     </row>
     <row r="47" spans="27:27" x14ac:dyDescent="0.2">
       <c r="AA47" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="48" spans="27:27" x14ac:dyDescent="0.2">
@@ -40289,7 +40093,7 @@
     <row r="56" spans="9:14" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="57" spans="9:14" x14ac:dyDescent="0.2">
       <c r="I57" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J57" s="18"/>
       <c r="K57" s="18"/>
@@ -40350,10 +40154,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>7</v>
@@ -40365,10 +40169,10 @@
         <v>9</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AC1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -40946,7 +40750,7 @@
         <v>0</v>
       </c>
       <c r="J16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M16" t="e">
         <f t="shared" si="2"/>
@@ -41028,7 +40832,7 @@
         <v>0</v>
       </c>
       <c r="J19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M19" t="e">
         <f t="shared" si="2"/>
@@ -41111,7 +40915,7 @@
         <v>0</v>
       </c>
       <c r="J22" s="14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M22" t="e">
         <f t="shared" si="2"/>
@@ -41139,7 +40943,7 @@
         <v>0</v>
       </c>
       <c r="J23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M23" t="e">
         <f t="shared" si="2"/>
@@ -41200,7 +41004,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="AB25" s="5" t="e">
-        <f t="shared" ref="AB3:AB57" si="4">LN(F25)</f>
+        <f t="shared" ref="AB25:AB57" si="4">LN(F25)</f>
         <v>#NUM!</v>
       </c>
       <c r="AC25" s="8"/>
@@ -41944,7 +41748,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="I57" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J57" s="18"/>
       <c r="K57" s="18"/>
@@ -42363,6 +42167,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="21343963-c43f-42a4-b0bc-b203e64410f4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100150C6E3A01A79A4BB6F66956A6120D17" ma:contentTypeVersion="10" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="675b3873b2b3a50285c27b6e2251c5ac">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="21343963-c43f-42a4-b0bc-b203e64410f4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2be159a6f8ccf448de399b2de905d627" ns3:_="">
     <xsd:import namespace="21343963-c43f-42a4-b0bc-b203e64410f4"/>
@@ -42544,24 +42365,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0E5A08E-764A-49CD-B663-0CFE39F0EF50}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="21343963-c43f-42a4-b0bc-b203e64410f4"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="21343963-c43f-42a4-b0bc-b203e64410f4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB974918-D618-4A8E-9BED-86443E84A1C9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D79C0675-5D5E-478C-BB62-C10AAF972813}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -42577,28 +42405,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB974918-D618-4A8E-9BED-86443E84A1C9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0E5A08E-764A-49CD-B663-0CFE39F0EF50}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="21343963-c43f-42a4-b0bc-b203e64410f4"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
finito di sistemare codice di log(I)/V, con colori e puniti,
</commit_message>
<xml_diff>
--- a/relazioni/esperienza_2/codici/Esperienza_2.xlsx
+++ b/relazioni/esperienza_2/codici/Esperienza_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alessiobrusini/Desktop/LABORATORIO-DI-ELETTROMAGNETISMO/relazioni/esperienza_2/codici/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A1CEFA6-7174-B641-BFF8-20D50D56E44E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C20C452-B955-994B-AC5F-F8207827DB35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="27100" windowHeight="15920" activeTab="5" xr2:uid="{9832D23C-5E2D-EB46-85A1-EE46353BB05C}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="27100" windowHeight="15920" activeTab="3" xr2:uid="{9832D23C-5E2D-EB46-85A1-EE46353BB05C}"/>
   </bookViews>
   <sheets>
     <sheet name="Temp_1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="24">
   <si>
     <t>n.</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>intercetta</t>
+  </si>
+  <si>
+    <t>l</t>
   </si>
 </sst>
 </file>
@@ -36916,8 +36919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF5D825E-8ABD-AB46-9243-4AAB60C8E7B6}">
   <dimension ref="A1:AC44"/>
   <sheetViews>
-    <sheetView zoomScale="58" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" zoomScale="58" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -37815,6 +37818,11 @@
       <c r="E24" s="19"/>
       <c r="F24" s="19"/>
       <c r="G24" s="19"/>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="K27" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="37" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G37" t="s">
@@ -39243,7 +39251,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{964810A6-0329-CE44-9434-FAE1DDC1CC77}">
   <dimension ref="A1:AC58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="61" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView topLeftCell="I1" zoomScale="61" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -42175,15 +42183,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100150C6E3A01A79A4BB6F66956A6120D17" ma:contentTypeVersion="10" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="675b3873b2b3a50285c27b6e2251c5ac">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="21343963-c43f-42a4-b0bc-b203e64410f4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2be159a6f8ccf448de399b2de905d627" ns3:_="">
     <xsd:import namespace="21343963-c43f-42a4-b0bc-b203e64410f4"/>
@@ -42365,6 +42364,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0E5A08E-764A-49CD-B663-0CFE39F0EF50}">
   <ds:schemaRefs>
@@ -42382,14 +42390,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB974918-D618-4A8E-9BED-86443E84A1C9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D79C0675-5D5E-478C-BB62-C10AAF972813}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -42405,4 +42405,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB974918-D618-4A8E-9BED-86443E84A1C9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
finti grafici principali, manca se volete farla quella della resistenza dinamica. Per il resto tutto bene
</commit_message>
<xml_diff>
--- a/relazioni/esperienza_2/codici/Esperienza_2.xlsx
+++ b/relazioni/esperienza_2/codici/Esperienza_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manue\Documents\UNIVERSITA'\II ANNO\LABORATORIO-DI-ELETTROMAGNETISMO\relazioni\esperienza_2\codici\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alessiobrusini/Desktop/LABORATORIO-DI-ELETTROMAGNETISMO/relazioni/esperienza_2/codici/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348DA382-7920-40FC-82D6-DDDE02160B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8307B01A-45D6-024D-8F05-099003716C05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="5" activeTab="7" xr2:uid="{9832D23C-5E2D-EB46-85A1-EE46353BB05C}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17480" activeTab="8" xr2:uid="{9832D23C-5E2D-EB46-85A1-EE46353BB05C}"/>
   </bookViews>
   <sheets>
     <sheet name="Temp_1" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Temp_6" sheetId="7" r:id="rId6"/>
     <sheet name="Pol_inv" sheetId="6" r:id="rId7"/>
     <sheet name="Sheet1" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet2" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="39">
   <si>
     <t>n.</t>
   </si>
@@ -142,12 +143,6 @@
     <t>x=qV/kTn</t>
   </si>
   <si>
-    <t>I scelta</t>
-  </si>
-  <si>
-    <t>ln (I scelta)</t>
-  </si>
-  <si>
     <t>q</t>
   </si>
   <si>
@@ -174,12 +169,22 @@
   <si>
     <t>V5</t>
   </si>
+  <si>
+    <t>I_scelta(A)</t>
+  </si>
+  <si>
+    <t>I_0</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
+  </numFmts>
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -241,8 +246,15 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -270,6 +282,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -363,7 +381,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -382,6 +400,17 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -390,7 +419,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="14">
     <dxf>
@@ -451,7 +480,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1234,7 +1263,7 @@
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1733,7 +1762,7 @@
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2464,7 +2493,7 @@
 <file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2878,7 +2907,7 @@
 <file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3387,7 +3416,7 @@
 <file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4199,7 +4228,7 @@
 <file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4673,7 +4702,7 @@
 <file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5214,7 +5243,7 @@
 <file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5769,7 +5798,7 @@
 <file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -6177,7 +6206,7 @@
 <file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -6741,7 +6770,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -7430,7 +7459,7 @@
 <file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -7955,7 +7984,7 @@
 <file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -8447,7 +8476,7 @@
 <file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -8831,7 +8860,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -9522,7 +9551,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -10176,7 +10205,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -10803,7 +10832,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -11283,7 +11312,7 @@
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -11813,7 +11842,7 @@
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -12392,7 +12421,7 @@
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -32231,15 +32260,15 @@
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="11.19921875" customWidth="1"/>
+    <col min="1" max="4" width="11.1640625" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.19921875" customWidth="1"/>
-    <col min="28" max="29" width="11.19921875" customWidth="1"/>
+    <col min="13" max="13" width="11.1640625" customWidth="1"/>
+    <col min="28" max="29" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="16.2" thickBot="1">
+    <row r="1" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -32277,7 +32306,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="16.2" thickBot="1">
+    <row r="2" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>0</v>
       </c>
@@ -32317,7 +32346,7 @@
       </c>
       <c r="AC2" s="6"/>
     </row>
-    <row r="3" spans="1:29" ht="16.2" thickBot="1">
+    <row r="3" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -32357,7 +32386,7 @@
       </c>
       <c r="AC3" s="8"/>
     </row>
-    <row r="4" spans="1:29" ht="16.2" thickBot="1">
+    <row r="4" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -32397,7 +32426,7 @@
       </c>
       <c r="AC4" s="6"/>
     </row>
-    <row r="5" spans="1:29" ht="16.2" thickBot="1">
+    <row r="5" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -32437,7 +32466,7 @@
       </c>
       <c r="AC5" s="8"/>
     </row>
-    <row r="6" spans="1:29" ht="16.2" thickBot="1">
+    <row r="6" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -32477,7 +32506,7 @@
       </c>
       <c r="AC6" s="6"/>
     </row>
-    <row r="7" spans="1:29" ht="16.2" thickBot="1">
+    <row r="7" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -32517,7 +32546,7 @@
       </c>
       <c r="AC7" s="8"/>
     </row>
-    <row r="8" spans="1:29" ht="16.2" thickBot="1">
+    <row r="8" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -32557,7 +32586,7 @@
       </c>
       <c r="AC8" s="6"/>
     </row>
-    <row r="9" spans="1:29" ht="16.2" thickBot="1">
+    <row r="9" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -32597,7 +32626,7 @@
       </c>
       <c r="AC9" s="8"/>
     </row>
-    <row r="10" spans="1:29" ht="16.2" thickBot="1">
+    <row r="10" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -32637,7 +32666,7 @@
       </c>
       <c r="AC10" s="6"/>
     </row>
-    <row r="11" spans="1:29" ht="16.2" thickBot="1">
+    <row r="11" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>9</v>
       </c>
@@ -32677,7 +32706,7 @@
       </c>
       <c r="AC11" s="8"/>
     </row>
-    <row r="12" spans="1:29" ht="16.2" thickBot="1">
+    <row r="12" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -32717,7 +32746,7 @@
       </c>
       <c r="AC12" s="6"/>
     </row>
-    <row r="13" spans="1:29" ht="16.2" thickBot="1">
+    <row r="13" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>11</v>
       </c>
@@ -32757,7 +32786,7 @@
       </c>
       <c r="AC13" s="8"/>
     </row>
-    <row r="14" spans="1:29" ht="16.2" thickBot="1">
+    <row r="14" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -32797,7 +32826,7 @@
       </c>
       <c r="AC14" s="6"/>
     </row>
-    <row r="15" spans="1:29" ht="16.2" thickBot="1">
+    <row r="15" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>13</v>
       </c>
@@ -32837,7 +32866,7 @@
       </c>
       <c r="AC15" s="8"/>
     </row>
-    <row r="16" spans="1:29" ht="16.2" thickBot="1">
+    <row r="16" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>14</v>
       </c>
@@ -32880,7 +32909,7 @@
       </c>
       <c r="AC16" s="6"/>
     </row>
-    <row r="17" spans="1:29" ht="18" thickBot="1">
+    <row r="17" spans="1:29" ht="19" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>15</v>
       </c>
@@ -32924,7 +32953,7 @@
       </c>
       <c r="AC17" s="8"/>
     </row>
-    <row r="18" spans="1:29" ht="16.2" thickBot="1">
+    <row r="18" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>16</v>
       </c>
@@ -32964,7 +32993,7 @@
       </c>
       <c r="AC18" s="6"/>
     </row>
-    <row r="19" spans="1:29" ht="16.2" thickBot="1">
+    <row r="19" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>17</v>
       </c>
@@ -33007,7 +33036,7 @@
       </c>
       <c r="AC19" s="8"/>
     </row>
-    <row r="20" spans="1:29" ht="17.399999999999999" thickBot="1">
+    <row r="20" spans="1:29" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>18</v>
       </c>
@@ -33051,7 +33080,7 @@
       </c>
       <c r="AC20" s="6"/>
     </row>
-    <row r="21" spans="1:29" ht="18" thickBot="1">
+    <row r="21" spans="1:29" ht="19" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>19</v>
       </c>
@@ -33092,7 +33121,7 @@
       </c>
       <c r="AC21" s="8"/>
     </row>
-    <row r="22" spans="1:29" ht="21" thickBot="1">
+    <row r="22" spans="1:29" ht="21" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>20</v>
       </c>
@@ -33135,7 +33164,7 @@
       </c>
       <c r="AC22" s="6"/>
     </row>
-    <row r="23" spans="1:29" ht="16.2" thickBot="1">
+    <row r="23" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>21</v>
       </c>
@@ -33178,7 +33207,7 @@
       </c>
       <c r="AC23" s="8"/>
     </row>
-    <row r="24" spans="1:29" ht="16.2" thickBot="1">
+    <row r="24" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>22</v>
       </c>
@@ -33218,7 +33247,7 @@
       </c>
       <c r="AC24" s="6"/>
     </row>
-    <row r="25" spans="1:29" ht="16.2" thickBot="1">
+    <row r="25" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>23</v>
       </c>
@@ -33258,7 +33287,7 @@
       </c>
       <c r="AC25" s="8"/>
     </row>
-    <row r="26" spans="1:29" ht="16.2" thickBot="1">
+    <row r="26" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>24</v>
       </c>
@@ -33298,7 +33327,7 @@
       </c>
       <c r="AC26" s="6"/>
     </row>
-    <row r="27" spans="1:29" ht="16.2" thickBot="1">
+    <row r="27" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>25</v>
       </c>
@@ -33338,7 +33367,7 @@
       </c>
       <c r="AC27" s="8"/>
     </row>
-    <row r="28" spans="1:29" ht="16.2" thickBot="1">
+    <row r="28" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>26</v>
       </c>
@@ -33378,7 +33407,7 @@
       </c>
       <c r="AC28" s="6"/>
     </row>
-    <row r="29" spans="1:29" ht="16.2" thickBot="1">
+    <row r="29" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>27</v>
       </c>
@@ -33418,7 +33447,7 @@
       </c>
       <c r="AC29" s="8"/>
     </row>
-    <row r="30" spans="1:29" ht="16.2" thickBot="1">
+    <row r="30" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>28</v>
       </c>
@@ -33458,7 +33487,7 @@
       </c>
       <c r="AC30" s="6"/>
     </row>
-    <row r="31" spans="1:29" ht="16.2" thickBot="1">
+    <row r="31" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>29</v>
       </c>
@@ -33498,7 +33527,7 @@
       </c>
       <c r="AC31" s="6"/>
     </row>
-    <row r="32" spans="1:29" ht="16.2" thickBot="1">
+    <row r="32" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>30</v>
       </c>
@@ -33538,7 +33567,7 @@
       </c>
       <c r="AC32" s="8"/>
     </row>
-    <row r="33" spans="1:29" ht="16.2" thickBot="1">
+    <row r="33" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>31</v>
       </c>
@@ -33578,7 +33607,7 @@
       </c>
       <c r="AC33" s="6"/>
     </row>
-    <row r="34" spans="1:29" ht="16.2" thickBot="1">
+    <row r="34" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>32</v>
       </c>
@@ -33618,7 +33647,7 @@
       </c>
       <c r="AC34" s="6"/>
     </row>
-    <row r="35" spans="1:29" ht="16.2" thickBot="1">
+    <row r="35" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <v>33</v>
       </c>
@@ -33658,7 +33687,7 @@
       </c>
       <c r="AC35" s="8"/>
     </row>
-    <row r="36" spans="1:29" ht="16.2" thickBot="1">
+    <row r="36" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>34</v>
       </c>
@@ -33698,7 +33727,7 @@
       </c>
       <c r="AC36" s="6"/>
     </row>
-    <row r="37" spans="1:29" ht="16.2" thickBot="1">
+    <row r="37" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <v>35</v>
       </c>
@@ -33738,7 +33767,7 @@
       </c>
       <c r="AC37" s="6"/>
     </row>
-    <row r="38" spans="1:29" ht="16.2" thickBot="1">
+    <row r="38" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>36</v>
       </c>
@@ -33778,7 +33807,7 @@
       </c>
       <c r="AC38" s="8"/>
     </row>
-    <row r="39" spans="1:29" ht="16.2" thickBot="1">
+    <row r="39" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <v>37</v>
       </c>
@@ -33818,7 +33847,7 @@
       </c>
       <c r="AC39" s="6"/>
     </row>
-    <row r="40" spans="1:29" ht="16.2" thickBot="1">
+    <row r="40" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>38</v>
       </c>
@@ -33858,7 +33887,7 @@
       </c>
       <c r="AC40" s="6"/>
     </row>
-    <row r="41" spans="1:29" ht="16.2" thickBot="1">
+    <row r="41" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>39</v>
       </c>
@@ -33898,7 +33927,7 @@
       </c>
       <c r="AC41" s="8"/>
     </row>
-    <row r="42" spans="1:29" ht="16.2" thickBot="1">
+    <row r="42" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>40</v>
       </c>
@@ -33938,7 +33967,7 @@
       </c>
       <c r="AC42" s="6"/>
     </row>
-    <row r="43" spans="1:29" ht="16.2" thickBot="1">
+    <row r="43" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
         <v>41</v>
       </c>
@@ -33978,7 +34007,7 @@
       </c>
       <c r="AC43" s="6"/>
     </row>
-    <row r="44" spans="1:29" ht="16.2" thickBot="1">
+    <row r="44" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>42</v>
       </c>
@@ -34018,7 +34047,7 @@
       </c>
       <c r="AC44" s="8"/>
     </row>
-    <row r="45" spans="1:29" ht="16.2" thickBot="1">
+    <row r="45" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
         <v>43</v>
       </c>
@@ -34058,7 +34087,7 @@
       </c>
       <c r="AC45" s="6"/>
     </row>
-    <row r="46" spans="1:29" ht="16.2" thickBot="1">
+    <row r="46" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>44</v>
       </c>
@@ -34098,7 +34127,7 @@
       </c>
       <c r="AC46" s="6"/>
     </row>
-    <row r="47" spans="1:29" ht="16.2" thickBot="1">
+    <row r="47" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
         <v>45</v>
       </c>
@@ -34138,7 +34167,7 @@
       </c>
       <c r="AC47" s="8"/>
     </row>
-    <row r="48" spans="1:29" ht="16.2" thickBot="1">
+    <row r="48" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>46</v>
       </c>
@@ -34178,7 +34207,7 @@
       </c>
       <c r="AC48" s="6"/>
     </row>
-    <row r="49" spans="1:29" ht="16.2" thickBot="1">
+    <row r="49" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
         <v>47</v>
       </c>
@@ -34218,7 +34247,7 @@
       </c>
       <c r="AC49" s="6"/>
     </row>
-    <row r="50" spans="1:29" ht="16.2" thickBot="1">
+    <row r="50" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>48</v>
       </c>
@@ -34258,7 +34287,7 @@
       </c>
       <c r="AC50" s="8"/>
     </row>
-    <row r="51" spans="1:29" ht="16.2" thickBot="1">
+    <row r="51" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>49</v>
       </c>
@@ -34298,7 +34327,7 @@
       </c>
       <c r="AC51" s="6"/>
     </row>
-    <row r="52" spans="1:29" ht="16.2" thickBot="1">
+    <row r="52" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>50</v>
       </c>
@@ -34338,7 +34367,7 @@
       </c>
       <c r="AC52" s="6"/>
     </row>
-    <row r="53" spans="1:29" ht="16.2" thickBot="1">
+    <row r="53" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="7">
         <v>51</v>
       </c>
@@ -34378,7 +34407,7 @@
       </c>
       <c r="AC53" s="8"/>
     </row>
-    <row r="54" spans="1:29" ht="16.2" thickBot="1">
+    <row r="54" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>52</v>
       </c>
@@ -34418,7 +34447,7 @@
       </c>
       <c r="AC54" s="6"/>
     </row>
-    <row r="55" spans="1:29" ht="16.2" thickBot="1">
+    <row r="55" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="7">
         <v>53</v>
       </c>
@@ -34458,7 +34487,7 @@
       </c>
       <c r="AC55" s="6"/>
     </row>
-    <row r="56" spans="1:29" ht="16.2" thickBot="1">
+    <row r="56" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>54</v>
       </c>
@@ -34498,7 +34527,7 @@
       </c>
       <c r="AC56" s="8"/>
     </row>
-    <row r="57" spans="1:29" ht="16.2" thickBot="1">
+    <row r="57" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7">
         <v>55</v>
       </c>
@@ -34538,7 +34567,7 @@
       </c>
       <c r="AC57" s="6"/>
     </row>
-    <row r="58" spans="1:29">
+    <row r="58" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A58" s="5">
         <v>56</v>
       </c>
@@ -34567,37 +34596,37 @@
       <c r="AB58" s="5"/>
       <c r="AC58" s="6"/>
     </row>
-    <row r="59" spans="1:29" ht="16.2" thickBot="1">
+    <row r="59" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="AB59" s="5"/>
       <c r="AC59" s="8"/>
     </row>
-    <row r="60" spans="1:29">
-      <c r="B60" s="18" t="s">
+    <row r="60" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="B60" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C60" s="18"/>
-      <c r="D60" s="18"/>
-      <c r="E60" s="18"/>
-      <c r="F60" s="18"/>
-      <c r="G60" s="18"/>
+      <c r="C60" s="23"/>
+      <c r="D60" s="23"/>
+      <c r="E60" s="23"/>
+      <c r="F60" s="23"/>
+      <c r="G60" s="23"/>
       <c r="AB60" s="5"/>
       <c r="AC60" s="6"/>
     </row>
-    <row r="61" spans="1:29">
-      <c r="B61" s="19"/>
-      <c r="C61" s="19"/>
-      <c r="D61" s="19"/>
-      <c r="E61" s="19"/>
-      <c r="F61" s="19"/>
-      <c r="G61" s="19"/>
+    <row r="61" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="B61" s="24"/>
+      <c r="C61" s="24"/>
+      <c r="D61" s="24"/>
+      <c r="E61" s="24"/>
+      <c r="F61" s="24"/>
+      <c r="G61" s="24"/>
       <c r="AB61" s="5"/>
       <c r="AC61" s="6"/>
     </row>
-    <row r="62" spans="1:29">
+    <row r="62" spans="1:29" x14ac:dyDescent="0.2">
       <c r="AB62" s="5"/>
       <c r="AC62" s="8"/>
     </row>
-    <row r="63" spans="1:29">
+    <row r="63" spans="1:29" x14ac:dyDescent="0.2">
       <c r="AB63" s="5"/>
       <c r="AC63" s="6"/>
     </row>
@@ -34618,19 +34647,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E64FDFDC-13B1-AB4C-B1C3-7FF9E2CAD166}">
   <dimension ref="A1:AC35"/>
   <sheetViews>
-    <sheetView topLeftCell="AA1" zoomScale="75" zoomScaleNormal="40" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="11.19921875" customWidth="1"/>
+    <col min="1" max="4" width="11.1640625" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.19921875" customWidth="1"/>
-    <col min="28" max="29" width="11.19921875" customWidth="1"/>
+    <col min="13" max="13" width="11.1640625" customWidth="1"/>
+    <col min="28" max="29" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="16.2" thickBot="1">
+    <row r="1" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -34668,7 +34697,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="16.2" thickBot="1">
+    <row r="2" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>0</v>
       </c>
@@ -34708,7 +34737,7 @@
       </c>
       <c r="AC2" s="6"/>
     </row>
-    <row r="3" spans="1:29" ht="16.2" thickBot="1">
+    <row r="3" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -34748,7 +34777,7 @@
       </c>
       <c r="AC3" s="8"/>
     </row>
-    <row r="4" spans="1:29" ht="16.2" thickBot="1">
+    <row r="4" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -34788,7 +34817,7 @@
       </c>
       <c r="AC4" s="6"/>
     </row>
-    <row r="5" spans="1:29" ht="16.2" thickBot="1">
+    <row r="5" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -34828,7 +34857,7 @@
       </c>
       <c r="AC5" s="8"/>
     </row>
-    <row r="6" spans="1:29" ht="16.2" thickBot="1">
+    <row r="6" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -34868,7 +34897,7 @@
       </c>
       <c r="AC6" s="6"/>
     </row>
-    <row r="7" spans="1:29" ht="16.2" thickBot="1">
+    <row r="7" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -34908,7 +34937,7 @@
       </c>
       <c r="AC7" s="8"/>
     </row>
-    <row r="8" spans="1:29" ht="16.2" thickBot="1">
+    <row r="8" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -34948,7 +34977,7 @@
       </c>
       <c r="AC8" s="6"/>
     </row>
-    <row r="9" spans="1:29" ht="16.2" thickBot="1">
+    <row r="9" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -34988,7 +35017,7 @@
       </c>
       <c r="AC9" s="8"/>
     </row>
-    <row r="10" spans="1:29" ht="16.2" thickBot="1">
+    <row r="10" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -35028,7 +35057,7 @@
       </c>
       <c r="AC10" s="6"/>
     </row>
-    <row r="11" spans="1:29" ht="16.2" thickBot="1">
+    <row r="11" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>9</v>
       </c>
@@ -35068,7 +35097,7 @@
       </c>
       <c r="AC11" s="8"/>
     </row>
-    <row r="12" spans="1:29" ht="16.2" thickBot="1">
+    <row r="12" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -35108,7 +35137,7 @@
       </c>
       <c r="AC12" s="6"/>
     </row>
-    <row r="13" spans="1:29" ht="16.2" thickBot="1">
+    <row r="13" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>11</v>
       </c>
@@ -35148,7 +35177,7 @@
       </c>
       <c r="AC13" s="8"/>
     </row>
-    <row r="14" spans="1:29" ht="16.2" thickBot="1">
+    <row r="14" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -35188,7 +35217,7 @@
       </c>
       <c r="AC14" s="6"/>
     </row>
-    <row r="15" spans="1:29" ht="16.2" thickBot="1">
+    <row r="15" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>13</v>
       </c>
@@ -35228,7 +35257,7 @@
       </c>
       <c r="AC15" s="8"/>
     </row>
-    <row r="16" spans="1:29" ht="16.2" thickBot="1">
+    <row r="16" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>14</v>
       </c>
@@ -35271,7 +35300,7 @@
       </c>
       <c r="AC16" s="6"/>
     </row>
-    <row r="17" spans="1:29" ht="18" thickBot="1">
+    <row r="17" spans="1:29" ht="19" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>15</v>
       </c>
@@ -35315,7 +35344,7 @@
       </c>
       <c r="AC17" s="8"/>
     </row>
-    <row r="18" spans="1:29" ht="16.2" thickBot="1">
+    <row r="18" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>16</v>
       </c>
@@ -35355,7 +35384,7 @@
       </c>
       <c r="AC18" s="6"/>
     </row>
-    <row r="19" spans="1:29" ht="16.2" thickBot="1">
+    <row r="19" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>17</v>
       </c>
@@ -35398,7 +35427,7 @@
       </c>
       <c r="AC19" s="8"/>
     </row>
-    <row r="20" spans="1:29" ht="17.399999999999999" thickBot="1">
+    <row r="20" spans="1:29" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>18</v>
       </c>
@@ -35442,7 +35471,7 @@
       </c>
       <c r="AC20" s="6"/>
     </row>
-    <row r="21" spans="1:29" ht="18" thickBot="1">
+    <row r="21" spans="1:29" ht="19" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>19</v>
       </c>
@@ -35483,7 +35512,7 @@
       </c>
       <c r="AC21" s="8"/>
     </row>
-    <row r="22" spans="1:29" ht="21" thickBot="1">
+    <row r="22" spans="1:29" ht="21" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>20</v>
       </c>
@@ -35526,7 +35555,7 @@
       </c>
       <c r="AC22" s="6"/>
     </row>
-    <row r="23" spans="1:29" ht="16.2" thickBot="1">
+    <row r="23" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>21</v>
       </c>
@@ -35569,7 +35598,7 @@
       </c>
       <c r="AC23" s="8"/>
     </row>
-    <row r="24" spans="1:29" ht="16.2" thickBot="1">
+    <row r="24" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>22</v>
       </c>
@@ -35609,7 +35638,7 @@
       </c>
       <c r="AC24" s="6"/>
     </row>
-    <row r="25" spans="1:29" ht="16.2" thickBot="1">
+    <row r="25" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>23</v>
       </c>
@@ -35649,7 +35678,7 @@
       </c>
       <c r="AC25" s="8"/>
     </row>
-    <row r="26" spans="1:29" ht="16.2" thickBot="1">
+    <row r="26" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>24</v>
       </c>
@@ -35689,7 +35718,7 @@
       </c>
       <c r="AC26" s="6"/>
     </row>
-    <row r="27" spans="1:29" ht="16.2" thickBot="1">
+    <row r="27" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>25</v>
       </c>
@@ -35729,7 +35758,7 @@
       </c>
       <c r="AC27" s="8"/>
     </row>
-    <row r="28" spans="1:29" ht="16.2" thickBot="1">
+    <row r="28" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>26</v>
       </c>
@@ -35769,7 +35798,7 @@
       </c>
       <c r="AC28" s="6"/>
     </row>
-    <row r="29" spans="1:29" ht="16.2" thickBot="1">
+    <row r="29" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>27</v>
       </c>
@@ -35809,7 +35838,7 @@
       </c>
       <c r="AC29" s="8"/>
     </row>
-    <row r="30" spans="1:29" ht="16.2" thickBot="1">
+    <row r="30" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>28</v>
       </c>
@@ -35849,7 +35878,7 @@
       </c>
       <c r="AC30" s="6"/>
     </row>
-    <row r="31" spans="1:29" ht="16.2" thickBot="1">
+    <row r="31" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>29</v>
       </c>
@@ -35889,7 +35918,7 @@
       </c>
       <c r="AC31" s="6"/>
     </row>
-    <row r="32" spans="1:29" ht="16.2" thickBot="1">
+    <row r="32" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>30</v>
       </c>
@@ -35916,24 +35945,24 @@
         <v>11.240110077866133</v>
       </c>
     </row>
-    <row r="33" spans="2:7" ht="16.2" thickBot="1"/>
-    <row r="34" spans="2:7">
-      <c r="B34" s="18" t="s">
+    <row r="33" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B34" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
     </row>
-    <row r="35" spans="2:7">
-      <c r="B35" s="19"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B35" s="24"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -35952,18 +35981,18 @@
   <dimension ref="A1:AC58"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="AB2" sqref="AB2"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="11.19921875" customWidth="1"/>
+    <col min="1" max="4" width="11.1640625" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.19921875" customWidth="1"/>
-    <col min="28" max="29" width="11.19921875" customWidth="1"/>
+    <col min="13" max="13" width="11.1640625" customWidth="1"/>
+    <col min="28" max="29" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="16.2" thickBot="1">
+    <row r="1" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -36001,7 +36030,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="16.2" thickBot="1">
+    <row r="2" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>0</v>
       </c>
@@ -36042,7 +36071,7 @@
       </c>
       <c r="AC2" s="6"/>
     </row>
-    <row r="3" spans="1:29" ht="16.2" thickBot="1">
+    <row r="3" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -36082,7 +36111,7 @@
       </c>
       <c r="AC3" s="8"/>
     </row>
-    <row r="4" spans="1:29" ht="16.2" thickBot="1">
+    <row r="4" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -36122,7 +36151,7 @@
       </c>
       <c r="AC4" s="6"/>
     </row>
-    <row r="5" spans="1:29" ht="16.2" thickBot="1">
+    <row r="5" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -36162,7 +36191,7 @@
       </c>
       <c r="AC5" s="8"/>
     </row>
-    <row r="6" spans="1:29" ht="16.2" thickBot="1">
+    <row r="6" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -36202,7 +36231,7 @@
       </c>
       <c r="AC6" s="6"/>
     </row>
-    <row r="7" spans="1:29" ht="16.2" thickBot="1">
+    <row r="7" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -36242,7 +36271,7 @@
       </c>
       <c r="AC7" s="8"/>
     </row>
-    <row r="8" spans="1:29" ht="16.2" thickBot="1">
+    <row r="8" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -36282,7 +36311,7 @@
       </c>
       <c r="AC8" s="6"/>
     </row>
-    <row r="9" spans="1:29" ht="16.2" thickBot="1">
+    <row r="9" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -36322,7 +36351,7 @@
       </c>
       <c r="AC9" s="8"/>
     </row>
-    <row r="10" spans="1:29" ht="16.2" thickBot="1">
+    <row r="10" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -36362,7 +36391,7 @@
       </c>
       <c r="AC10" s="6"/>
     </row>
-    <row r="11" spans="1:29" ht="16.2" thickBot="1">
+    <row r="11" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>9</v>
       </c>
@@ -36402,7 +36431,7 @@
       </c>
       <c r="AC11" s="8"/>
     </row>
-    <row r="12" spans="1:29" ht="16.2" thickBot="1">
+    <row r="12" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -36442,7 +36471,7 @@
       </c>
       <c r="AC12" s="6"/>
     </row>
-    <row r="13" spans="1:29" ht="16.2" thickBot="1">
+    <row r="13" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>11</v>
       </c>
@@ -36482,7 +36511,7 @@
       </c>
       <c r="AC13" s="8"/>
     </row>
-    <row r="14" spans="1:29" ht="16.2" thickBot="1">
+    <row r="14" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -36522,7 +36551,7 @@
       </c>
       <c r="AC14" s="6"/>
     </row>
-    <row r="15" spans="1:29" ht="16.2" thickBot="1">
+    <row r="15" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>13</v>
       </c>
@@ -36562,7 +36591,7 @@
       </c>
       <c r="AC15" s="8"/>
     </row>
-    <row r="16" spans="1:29" ht="16.2" thickBot="1">
+    <row r="16" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>14</v>
       </c>
@@ -36605,7 +36634,7 @@
       </c>
       <c r="AC16" s="6"/>
     </row>
-    <row r="17" spans="1:29" ht="18" thickBot="1">
+    <row r="17" spans="1:29" ht="19" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>15</v>
       </c>
@@ -36649,7 +36678,7 @@
       </c>
       <c r="AC17" s="8"/>
     </row>
-    <row r="18" spans="1:29" ht="16.2" thickBot="1">
+    <row r="18" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>16</v>
       </c>
@@ -36689,7 +36718,7 @@
       </c>
       <c r="AC18" s="6"/>
     </row>
-    <row r="19" spans="1:29" ht="16.2" thickBot="1">
+    <row r="19" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>17</v>
       </c>
@@ -36732,7 +36761,7 @@
       </c>
       <c r="AC19" s="8"/>
     </row>
-    <row r="20" spans="1:29" ht="17.399999999999999" thickBot="1">
+    <row r="20" spans="1:29" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>18</v>
       </c>
@@ -36776,7 +36805,7 @@
       </c>
       <c r="AC20" s="6"/>
     </row>
-    <row r="21" spans="1:29" ht="18" thickBot="1">
+    <row r="21" spans="1:29" ht="19" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>19</v>
       </c>
@@ -36817,7 +36846,7 @@
       </c>
       <c r="AC21" s="8"/>
     </row>
-    <row r="22" spans="1:29" ht="21" thickBot="1">
+    <row r="22" spans="1:29" ht="21" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>20</v>
       </c>
@@ -36860,7 +36889,7 @@
       </c>
       <c r="AC22" s="6"/>
     </row>
-    <row r="23" spans="1:29" ht="16.2" thickBot="1">
+    <row r="23" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>21</v>
       </c>
@@ -36903,7 +36932,7 @@
       </c>
       <c r="AC23" s="8"/>
     </row>
-    <row r="24" spans="1:29" ht="16.2" thickBot="1">
+    <row r="24" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>22</v>
       </c>
@@ -36930,24 +36959,24 @@
         <v>13.466910915437513</v>
       </c>
     </row>
-    <row r="56" spans="9:14" ht="16.2" thickBot="1"/>
-    <row r="57" spans="9:14">
-      <c r="I57" s="18" t="s">
+    <row r="56" spans="9:14" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I57" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="J57" s="18"/>
-      <c r="K57" s="18"/>
-      <c r="L57" s="18"/>
-      <c r="M57" s="18"/>
-      <c r="N57" s="18"/>
+      <c r="J57" s="23"/>
+      <c r="K57" s="23"/>
+      <c r="L57" s="23"/>
+      <c r="M57" s="23"/>
+      <c r="N57" s="23"/>
     </row>
-    <row r="58" spans="9:14">
-      <c r="I58" s="19"/>
-      <c r="J58" s="19"/>
-      <c r="K58" s="19"/>
-      <c r="L58" s="19"/>
-      <c r="M58" s="19"/>
-      <c r="N58" s="19"/>
+    <row r="58" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I58" s="24"/>
+      <c r="J58" s="24"/>
+      <c r="K58" s="24"/>
+      <c r="L58" s="24"/>
+      <c r="M58" s="24"/>
+      <c r="N58" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -36969,19 +36998,19 @@
       <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="11.19921875" customWidth="1"/>
-    <col min="6" max="6" width="11.296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.19921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="4" width="11.1640625" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.19921875" customWidth="1"/>
-    <col min="14" max="14" width="11.296875" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="11.19921875" customWidth="1"/>
+    <col min="13" max="13" width="11.1640625" customWidth="1"/>
+    <col min="14" max="14" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="16.2" thickBot="1">
+    <row r="1" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -37019,7 +37048,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="16.2" thickBot="1">
+    <row r="2" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>0</v>
       </c>
@@ -37061,7 +37090,7 @@
       </c>
       <c r="AC2" s="6"/>
     </row>
-    <row r="3" spans="1:29" ht="16.2" thickBot="1">
+    <row r="3" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -37103,7 +37132,7 @@
       </c>
       <c r="AC3" s="8"/>
     </row>
-    <row r="4" spans="1:29" ht="16.2" thickBot="1">
+    <row r="4" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -37145,7 +37174,7 @@
       </c>
       <c r="AC4" s="6"/>
     </row>
-    <row r="5" spans="1:29" ht="16.2" thickBot="1">
+    <row r="5" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -37187,7 +37216,7 @@
       </c>
       <c r="AC5" s="8"/>
     </row>
-    <row r="6" spans="1:29" ht="16.2" thickBot="1">
+    <row r="6" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -37229,7 +37258,7 @@
       </c>
       <c r="AC6" s="6"/>
     </row>
-    <row r="7" spans="1:29" ht="16.2" thickBot="1">
+    <row r="7" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -37271,7 +37300,7 @@
       </c>
       <c r="AC7" s="8"/>
     </row>
-    <row r="8" spans="1:29" ht="16.2" thickBot="1">
+    <row r="8" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -37313,7 +37342,7 @@
       </c>
       <c r="AC8" s="6"/>
     </row>
-    <row r="9" spans="1:29" ht="16.2" thickBot="1">
+    <row r="9" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -37355,7 +37384,7 @@
       </c>
       <c r="AC9" s="8"/>
     </row>
-    <row r="10" spans="1:29" ht="16.2" thickBot="1">
+    <row r="10" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -37397,7 +37426,7 @@
       </c>
       <c r="AC10" s="6"/>
     </row>
-    <row r="11" spans="1:29" ht="16.2" thickBot="1">
+    <row r="11" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>9</v>
       </c>
@@ -37439,7 +37468,7 @@
       </c>
       <c r="AC11" s="8"/>
     </row>
-    <row r="12" spans="1:29" ht="16.2" thickBot="1">
+    <row r="12" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -37481,7 +37510,7 @@
       </c>
       <c r="AC12" s="6"/>
     </row>
-    <row r="13" spans="1:29" ht="16.2" thickBot="1">
+    <row r="13" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>11</v>
       </c>
@@ -37523,7 +37552,7 @@
       </c>
       <c r="AC13" s="8"/>
     </row>
-    <row r="14" spans="1:29" ht="16.2" thickBot="1">
+    <row r="14" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -37565,7 +37594,7 @@
       </c>
       <c r="AC14" s="6"/>
     </row>
-    <row r="15" spans="1:29" ht="16.2" thickBot="1">
+    <row r="15" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>13</v>
       </c>
@@ -37607,7 +37636,7 @@
       </c>
       <c r="AC15" s="8"/>
     </row>
-    <row r="16" spans="1:29" ht="16.2" thickBot="1">
+    <row r="16" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>14</v>
       </c>
@@ -37649,7 +37678,7 @@
       </c>
       <c r="AC16" s="6"/>
     </row>
-    <row r="17" spans="1:29" ht="16.2" thickBot="1">
+    <row r="17" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>15</v>
       </c>
@@ -37691,7 +37720,7 @@
       </c>
       <c r="AC17" s="8"/>
     </row>
-    <row r="18" spans="1:29" ht="16.2" thickBot="1">
+    <row r="18" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>16</v>
       </c>
@@ -37733,7 +37762,7 @@
       </c>
       <c r="AC18" s="6"/>
     </row>
-    <row r="19" spans="1:29" ht="16.2" thickBot="1">
+    <row r="19" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>17</v>
       </c>
@@ -37775,7 +37804,7 @@
       </c>
       <c r="AC19" s="8"/>
     </row>
-    <row r="20" spans="1:29" ht="16.2" thickBot="1">
+    <row r="20" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>18</v>
       </c>
@@ -37817,7 +37846,7 @@
       </c>
       <c r="AC20" s="6"/>
     </row>
-    <row r="21" spans="1:29">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
         <v>19</v>
       </c>
@@ -37846,61 +37875,61 @@
         <v>1.9813326740246377E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:29" ht="16.2" thickBot="1"/>
-    <row r="23" spans="1:29">
-      <c r="B23" s="18" t="s">
+    <row r="22" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="B23" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
     </row>
-    <row r="24" spans="1:29">
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
     </row>
-    <row r="27" spans="1:29">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
       <c r="K27" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="7:7">
+    <row r="37" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G37" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="7:7" ht="17.399999999999999">
+    <row r="38" spans="7:7" ht="18" x14ac:dyDescent="0.2">
       <c r="G38" s="9">
         <f>1.602176634*10^(-19)</f>
         <v>1.6021766340000001E-19</v>
       </c>
     </row>
-    <row r="40" spans="7:7">
+    <row r="40" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G40" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="7:7" ht="16.8">
+    <row r="41" spans="7:7" ht="17" x14ac:dyDescent="0.2">
       <c r="G41" s="11">
         <f>1.3806503*10^(-23)</f>
         <v>1.3806503000000004E-23</v>
       </c>
     </row>
-    <row r="42" spans="7:7" ht="17.399999999999999">
+    <row r="42" spans="7:7" ht="18" x14ac:dyDescent="0.2">
       <c r="G42" s="10"/>
     </row>
-    <row r="43" spans="7:7" ht="20.399999999999999">
+    <row r="43" spans="7:7" ht="20" x14ac:dyDescent="0.2">
       <c r="G43" s="14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="7:7">
+    <row r="44" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G44" t="s">
         <v>14</v>
       </c>
@@ -37921,22 +37950,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29EA75CD-2EAA-AD46-B54B-F32D80398925}">
   <dimension ref="A1:AC50"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" zoomScale="75" zoomScaleNormal="40" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="11.19921875" customWidth="1"/>
-    <col min="6" max="6" width="11.296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.69921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="4" width="11.1640625" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.19921875" customWidth="1"/>
-    <col min="14" max="14" width="11.296875" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="11.19921875" customWidth="1"/>
+    <col min="13" max="13" width="11.1640625" customWidth="1"/>
+    <col min="14" max="14" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="16.2" thickBot="1">
+    <row r="1" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -37980,7 +38009,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="16.2" thickBot="1">
+    <row r="2" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>0</v>
       </c>
@@ -38022,7 +38051,7 @@
       </c>
       <c r="AC2" s="6"/>
     </row>
-    <row r="3" spans="1:29" ht="16.2" thickBot="1">
+    <row r="3" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -38064,7 +38093,7 @@
       </c>
       <c r="AC3" s="8"/>
     </row>
-    <row r="4" spans="1:29" ht="16.2" thickBot="1">
+    <row r="4" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -38106,7 +38135,7 @@
       </c>
       <c r="AC4" s="6"/>
     </row>
-    <row r="5" spans="1:29" ht="16.2" thickBot="1">
+    <row r="5" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -38148,7 +38177,7 @@
       </c>
       <c r="AC5" s="8"/>
     </row>
-    <row r="6" spans="1:29" ht="16.2" thickBot="1">
+    <row r="6" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -38190,7 +38219,7 @@
       </c>
       <c r="AC6" s="6"/>
     </row>
-    <row r="7" spans="1:29" ht="16.2" thickBot="1">
+    <row r="7" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -38232,7 +38261,7 @@
       </c>
       <c r="AC7" s="8"/>
     </row>
-    <row r="8" spans="1:29" ht="16.2" thickBot="1">
+    <row r="8" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -38274,7 +38303,7 @@
       </c>
       <c r="AC8" s="6"/>
     </row>
-    <row r="9" spans="1:29" ht="16.2" thickBot="1">
+    <row r="9" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -38316,7 +38345,7 @@
       </c>
       <c r="AC9" s="8"/>
     </row>
-    <row r="10" spans="1:29" ht="16.2" thickBot="1">
+    <row r="10" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -38358,7 +38387,7 @@
       </c>
       <c r="AC10" s="6"/>
     </row>
-    <row r="11" spans="1:29" ht="16.2" thickBot="1">
+    <row r="11" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>9</v>
       </c>
@@ -38400,7 +38429,7 @@
       </c>
       <c r="AC11" s="8"/>
     </row>
-    <row r="12" spans="1:29" ht="16.2" thickBot="1">
+    <row r="12" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -38442,7 +38471,7 @@
       </c>
       <c r="AC12" s="6"/>
     </row>
-    <row r="13" spans="1:29" ht="16.2" thickBot="1">
+    <row r="13" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>11</v>
       </c>
@@ -38484,7 +38513,7 @@
       </c>
       <c r="AC13" s="8"/>
     </row>
-    <row r="14" spans="1:29" ht="16.2" thickBot="1">
+    <row r="14" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -38526,7 +38555,7 @@
       </c>
       <c r="AC14" s="6"/>
     </row>
-    <row r="15" spans="1:29" ht="16.2" thickBot="1">
+    <row r="15" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>13</v>
       </c>
@@ -38568,7 +38597,7 @@
       </c>
       <c r="AC15" s="8"/>
     </row>
-    <row r="16" spans="1:29" ht="16.2" thickBot="1">
+    <row r="16" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>14</v>
       </c>
@@ -38610,7 +38639,7 @@
       </c>
       <c r="AC16" s="6"/>
     </row>
-    <row r="17" spans="1:29" ht="16.2" thickBot="1">
+    <row r="17" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>15</v>
       </c>
@@ -38652,7 +38681,7 @@
       </c>
       <c r="AC17" s="8"/>
     </row>
-    <row r="18" spans="1:29" ht="16.2" thickBot="1">
+    <row r="18" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>16</v>
       </c>
@@ -38694,7 +38723,7 @@
       </c>
       <c r="AC18" s="6"/>
     </row>
-    <row r="19" spans="1:29" ht="16.2" thickBot="1">
+    <row r="19" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>17</v>
       </c>
@@ -38736,7 +38765,7 @@
       </c>
       <c r="AC19" s="8"/>
     </row>
-    <row r="20" spans="1:29" ht="16.2" thickBot="1">
+    <row r="20" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>18</v>
       </c>
@@ -38778,7 +38807,7 @@
       </c>
       <c r="AC20" s="6"/>
     </row>
-    <row r="21" spans="1:29" ht="16.2" thickBot="1">
+    <row r="21" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>19</v>
       </c>
@@ -38820,7 +38849,7 @@
       </c>
       <c r="AC21" s="8"/>
     </row>
-    <row r="22" spans="1:29" ht="16.2" thickBot="1">
+    <row r="22" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>20</v>
       </c>
@@ -38862,7 +38891,7 @@
       </c>
       <c r="AC22" s="6"/>
     </row>
-    <row r="23" spans="1:29" ht="16.2" thickBot="1">
+    <row r="23" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>21</v>
       </c>
@@ -38904,7 +38933,7 @@
       </c>
       <c r="AC23" s="8"/>
     </row>
-    <row r="24" spans="1:29" ht="16.2" thickBot="1">
+    <row r="24" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>22</v>
       </c>
@@ -38946,7 +38975,7 @@
       </c>
       <c r="AC24" s="6"/>
     </row>
-    <row r="25" spans="1:29" ht="16.2" thickBot="1">
+    <row r="25" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>23</v>
       </c>
@@ -38988,7 +39017,7 @@
       </c>
       <c r="AC25" s="8"/>
     </row>
-    <row r="26" spans="1:29" ht="16.2" thickBot="1">
+    <row r="26" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>24</v>
       </c>
@@ -39030,7 +39059,7 @@
       </c>
       <c r="AC26" s="6"/>
     </row>
-    <row r="27" spans="1:29" ht="16.2" thickBot="1">
+    <row r="27" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>25</v>
       </c>
@@ -39072,7 +39101,7 @@
       </c>
       <c r="AC27" s="8"/>
     </row>
-    <row r="28" spans="1:29" ht="16.2" thickBot="1">
+    <row r="28" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>26</v>
       </c>
@@ -39114,7 +39143,7 @@
       </c>
       <c r="AC28" s="6"/>
     </row>
-    <row r="29" spans="1:29" ht="16.2" thickBot="1">
+    <row r="29" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>27</v>
       </c>
@@ -39156,7 +39185,7 @@
       </c>
       <c r="AC29" s="8"/>
     </row>
-    <row r="30" spans="1:29" ht="16.2" thickBot="1">
+    <row r="30" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>28</v>
       </c>
@@ -39198,7 +39227,7 @@
       </c>
       <c r="AC30" s="6"/>
     </row>
-    <row r="31" spans="1:29">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A31" s="7">
         <v>29</v>
       </c>
@@ -39227,56 +39256,56 @@
         <v>6.6325231377546354E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:29" ht="16.2" thickBot="1"/>
-    <row r="33" spans="2:8">
-      <c r="B33" s="18" t="s">
+    <row r="32" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B33" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
     </row>
-    <row r="34" spans="2:8">
-      <c r="B34" s="19"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B34" s="24"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
     </row>
-    <row r="43" spans="2:8">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
       <c r="H43" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="2:8" ht="17.399999999999999">
+    <row r="44" spans="2:8" ht="18" x14ac:dyDescent="0.2">
       <c r="H44" s="9">
         <f>1.602176634*10^(-19)</f>
         <v>1.6021766340000001E-19</v>
       </c>
     </row>
-    <row r="46" spans="2:8">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
       <c r="H46" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="2:8" ht="16.8">
+    <row r="47" spans="2:8" ht="17" x14ac:dyDescent="0.2">
       <c r="H47" s="11">
         <f>1.3806503*10^(-23)</f>
         <v>1.3806503000000004E-23</v>
       </c>
     </row>
-    <row r="48" spans="2:8" ht="17.399999999999999">
+    <row r="48" spans="2:8" ht="18" x14ac:dyDescent="0.2">
       <c r="H48" s="10"/>
     </row>
-    <row r="49" spans="8:8" ht="20.399999999999999">
+    <row r="49" spans="8:8" ht="20" x14ac:dyDescent="0.2">
       <c r="H49" s="14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="8:8">
+    <row r="50" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H50" t="s">
         <v>14</v>
       </c>
@@ -39298,18 +39327,18 @@
   <dimension ref="A1:AC58"/>
   <sheetViews>
     <sheetView zoomScale="61" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="11.19921875" customWidth="1"/>
+    <col min="1" max="4" width="11.1640625" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.19921875" customWidth="1"/>
-    <col min="28" max="29" width="11.19921875" customWidth="1"/>
+    <col min="13" max="13" width="11.1640625" customWidth="1"/>
+    <col min="28" max="29" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="16.2" thickBot="1">
+    <row r="1" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -39347,7 +39376,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="16.2" thickBot="1">
+    <row r="2" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>0</v>
       </c>
@@ -39388,7 +39417,7 @@
       </c>
       <c r="AC2" s="6"/>
     </row>
-    <row r="3" spans="1:29" ht="16.2" thickBot="1">
+    <row r="3" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -39429,7 +39458,7 @@
       </c>
       <c r="AC3" s="8"/>
     </row>
-    <row r="4" spans="1:29" ht="16.2" thickBot="1">
+    <row r="4" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -39470,7 +39499,7 @@
       </c>
       <c r="AC4" s="6"/>
     </row>
-    <row r="5" spans="1:29" ht="16.2" thickBot="1">
+    <row r="5" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -39511,7 +39540,7 @@
       </c>
       <c r="AC5" s="8"/>
     </row>
-    <row r="6" spans="1:29" ht="16.2" thickBot="1">
+    <row r="6" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -39552,7 +39581,7 @@
       </c>
       <c r="AC6" s="6"/>
     </row>
-    <row r="7" spans="1:29" ht="16.2" thickBot="1">
+    <row r="7" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -39593,7 +39622,7 @@
       </c>
       <c r="AC7" s="8"/>
     </row>
-    <row r="8" spans="1:29" ht="16.2" thickBot="1">
+    <row r="8" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -39634,7 +39663,7 @@
       </c>
       <c r="AC8" s="6"/>
     </row>
-    <row r="9" spans="1:29" ht="16.2" thickBot="1">
+    <row r="9" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -39675,7 +39704,7 @@
       </c>
       <c r="AC9" s="8"/>
     </row>
-    <row r="10" spans="1:29" ht="16.2" thickBot="1">
+    <row r="10" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -39716,7 +39745,7 @@
       </c>
       <c r="AC10" s="6"/>
     </row>
-    <row r="11" spans="1:29" ht="16.2" thickBot="1">
+    <row r="11" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>9</v>
       </c>
@@ -39757,7 +39786,7 @@
       </c>
       <c r="AC11" s="8"/>
     </row>
-    <row r="12" spans="1:29" ht="16.2" thickBot="1">
+    <row r="12" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -39798,7 +39827,7 @@
       </c>
       <c r="AC12" s="6"/>
     </row>
-    <row r="13" spans="1:29" ht="16.2" thickBot="1">
+    <row r="13" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>11</v>
       </c>
@@ -39839,7 +39868,7 @@
       </c>
       <c r="AC13" s="8"/>
     </row>
-    <row r="14" spans="1:29" ht="16.2" thickBot="1">
+    <row r="14" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -39880,7 +39909,7 @@
       </c>
       <c r="AC14" s="6"/>
     </row>
-    <row r="15" spans="1:29" ht="16.2" thickBot="1">
+    <row r="15" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>13</v>
       </c>
@@ -39921,7 +39950,7 @@
       </c>
       <c r="AC15" s="8"/>
     </row>
-    <row r="16" spans="1:29" ht="16.2" thickBot="1">
+    <row r="16" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>14</v>
       </c>
@@ -39965,7 +39994,7 @@
       </c>
       <c r="AC16" s="6"/>
     </row>
-    <row r="17" spans="1:29" ht="18" thickBot="1">
+    <row r="17" spans="1:29" ht="19" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>15</v>
       </c>
@@ -40010,7 +40039,7 @@
       </c>
       <c r="AC17" s="8"/>
     </row>
-    <row r="18" spans="1:29" ht="16.2" thickBot="1">
+    <row r="18" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>16</v>
       </c>
@@ -40051,7 +40080,7 @@
       </c>
       <c r="AC18" s="6"/>
     </row>
-    <row r="19" spans="1:29" ht="16.2" thickBot="1">
+    <row r="19" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>17</v>
       </c>
@@ -40095,7 +40124,7 @@
       </c>
       <c r="AC19" s="8"/>
     </row>
-    <row r="20" spans="1:29" ht="17.399999999999999" thickBot="1">
+    <row r="20" spans="1:29" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>18</v>
       </c>
@@ -40128,59 +40157,59 @@
       </c>
       <c r="AB20" s="5"/>
     </row>
-    <row r="21" spans="1:29" ht="17.399999999999999">
+    <row r="21" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="J21" s="10"/>
     </row>
-    <row r="22" spans="1:29" ht="20.399999999999999">
+    <row r="22" spans="1:29" ht="20" x14ac:dyDescent="0.2">
       <c r="J22" s="14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:29">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
       <c r="J23" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="27:27">
+    <row r="44" spans="27:27" x14ac:dyDescent="0.2">
       <c r="AA44" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="27:27">
+    <row r="45" spans="27:27" x14ac:dyDescent="0.2">
       <c r="AA45">
         <f>SLOPE(AB2:AB19,H2:H19)</f>
         <v>0.55845473451013328</v>
       </c>
     </row>
-    <row r="47" spans="27:27">
+    <row r="47" spans="27:27" x14ac:dyDescent="0.2">
       <c r="AA47" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="27:27">
+    <row r="48" spans="27:27" x14ac:dyDescent="0.2">
       <c r="AA48">
         <f>INTERCEPT(AB2:AB19,H2:H19)</f>
         <v>-93.280856724131766</v>
       </c>
     </row>
-    <row r="56" spans="9:14" ht="16.2" thickBot="1"/>
-    <row r="57" spans="9:14">
-      <c r="I57" s="18" t="s">
+    <row r="56" spans="9:14" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I57" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="J57" s="18"/>
-      <c r="K57" s="18"/>
-      <c r="L57" s="18"/>
-      <c r="M57" s="18"/>
-      <c r="N57" s="18"/>
+      <c r="J57" s="23"/>
+      <c r="K57" s="23"/>
+      <c r="L57" s="23"/>
+      <c r="M57" s="23"/>
+      <c r="N57" s="23"/>
     </row>
-    <row r="58" spans="9:14">
-      <c r="I58" s="19"/>
-      <c r="J58" s="19"/>
-      <c r="K58" s="19"/>
-      <c r="L58" s="19"/>
-      <c r="M58" s="19"/>
-      <c r="N58" s="19"/>
+    <row r="58" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I58" s="24"/>
+      <c r="J58" s="24"/>
+      <c r="K58" s="24"/>
+      <c r="L58" s="24"/>
+      <c r="M58" s="24"/>
+      <c r="N58" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -40202,15 +40231,15 @@
       <selection activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="11.19921875" customWidth="1"/>
+    <col min="1" max="4" width="11.1640625" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.19921875" customWidth="1"/>
-    <col min="28" max="29" width="11.19921875" customWidth="1"/>
+    <col min="13" max="13" width="11.1640625" customWidth="1"/>
+    <col min="28" max="29" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="16.2" thickBot="1">
+    <row r="1" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -40248,7 +40277,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="16.2" thickBot="1">
+    <row r="2" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>0</v>
       </c>
@@ -40288,7 +40317,7 @@
       </c>
       <c r="AC2" s="6"/>
     </row>
-    <row r="3" spans="1:29" ht="16.2" thickBot="1">
+    <row r="3" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -40328,7 +40357,7 @@
       </c>
       <c r="AC3" s="8"/>
     </row>
-    <row r="4" spans="1:29" ht="16.2" thickBot="1">
+    <row r="4" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -40368,7 +40397,7 @@
       </c>
       <c r="AC4" s="6"/>
     </row>
-    <row r="5" spans="1:29" ht="16.2" thickBot="1">
+    <row r="5" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -40408,7 +40437,7 @@
       </c>
       <c r="AC5" s="8"/>
     </row>
-    <row r="6" spans="1:29" ht="16.2" thickBot="1">
+    <row r="6" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -40448,7 +40477,7 @@
       </c>
       <c r="AC6" s="6"/>
     </row>
-    <row r="7" spans="1:29" ht="16.2" thickBot="1">
+    <row r="7" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -40488,7 +40517,7 @@
       </c>
       <c r="AC7" s="8"/>
     </row>
-    <row r="8" spans="1:29" ht="16.2" thickBot="1">
+    <row r="8" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -40528,7 +40557,7 @@
       </c>
       <c r="AC8" s="6"/>
     </row>
-    <row r="9" spans="1:29" ht="16.2" thickBot="1">
+    <row r="9" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -40568,7 +40597,7 @@
       </c>
       <c r="AC9" s="8"/>
     </row>
-    <row r="10" spans="1:29" ht="16.2" thickBot="1">
+    <row r="10" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -40608,7 +40637,7 @@
       </c>
       <c r="AC10" s="6"/>
     </row>
-    <row r="11" spans="1:29" ht="16.2" thickBot="1">
+    <row r="11" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>9</v>
       </c>
@@ -40648,7 +40677,7 @@
       </c>
       <c r="AC11" s="8"/>
     </row>
-    <row r="12" spans="1:29" ht="16.2" thickBot="1">
+    <row r="12" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -40688,7 +40717,7 @@
       </c>
       <c r="AC12" s="6"/>
     </row>
-    <row r="13" spans="1:29" ht="16.2" thickBot="1">
+    <row r="13" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>11</v>
       </c>
@@ -40728,7 +40757,7 @@
       </c>
       <c r="AC13" s="8"/>
     </row>
-    <row r="14" spans="1:29" ht="16.2" thickBot="1">
+    <row r="14" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -40768,7 +40797,7 @@
       </c>
       <c r="AC14" s="6"/>
     </row>
-    <row r="15" spans="1:29" ht="16.2" thickBot="1">
+    <row r="15" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>13</v>
       </c>
@@ -40808,7 +40837,7 @@
       </c>
       <c r="AC15" s="8"/>
     </row>
-    <row r="16" spans="1:29" ht="16.2" thickBot="1">
+    <row r="16" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>14</v>
       </c>
@@ -40836,7 +40865,7 @@
       <c r="AB16" s="5"/>
       <c r="AC16" s="6"/>
     </row>
-    <row r="17" spans="1:29" ht="18" thickBot="1">
+    <row r="17" spans="1:29" ht="19" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>15</v>
       </c>
@@ -40865,7 +40894,7 @@
       <c r="AB17" s="5"/>
       <c r="AC17" s="8"/>
     </row>
-    <row r="18" spans="1:29" ht="16.2" thickBot="1">
+    <row r="18" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>16</v>
       </c>
@@ -40890,7 +40919,7 @@
       <c r="AB18" s="5"/>
       <c r="AC18" s="6"/>
     </row>
-    <row r="19" spans="1:29" ht="16.2" thickBot="1">
+    <row r="19" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>17</v>
       </c>
@@ -40918,7 +40947,7 @@
       <c r="AB19" s="5"/>
       <c r="AC19" s="8"/>
     </row>
-    <row r="20" spans="1:29" ht="17.399999999999999" thickBot="1">
+    <row r="20" spans="1:29" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>18</v>
       </c>
@@ -40947,7 +40976,7 @@
       <c r="AB20" s="5"/>
       <c r="AC20" s="6"/>
     </row>
-    <row r="21" spans="1:29" ht="18" thickBot="1">
+    <row r="21" spans="1:29" ht="19" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>19</v>
       </c>
@@ -40973,7 +41002,7 @@
       <c r="AB21" s="5"/>
       <c r="AC21" s="8"/>
     </row>
-    <row r="22" spans="1:29" ht="21" thickBot="1">
+    <row r="22" spans="1:29" ht="21" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>20</v>
       </c>
@@ -41001,7 +41030,7 @@
       <c r="AB22" s="5"/>
       <c r="AC22" s="6"/>
     </row>
-    <row r="23" spans="1:29" ht="16.2" thickBot="1">
+    <row r="23" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>21</v>
       </c>
@@ -41029,7 +41058,7 @@
       <c r="AB23" s="5"/>
       <c r="AC23" s="8"/>
     </row>
-    <row r="24" spans="1:29" ht="16.2" thickBot="1">
+    <row r="24" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>22</v>
       </c>
@@ -41054,7 +41083,7 @@
       <c r="AB24" s="5"/>
       <c r="AC24" s="6"/>
     </row>
-    <row r="25" spans="1:29" ht="16.2" thickBot="1">
+    <row r="25" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>23</v>
       </c>
@@ -41082,7 +41111,7 @@
       </c>
       <c r="AC25" s="8"/>
     </row>
-    <row r="26" spans="1:29" ht="16.2" thickBot="1">
+    <row r="26" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>24</v>
       </c>
@@ -41110,7 +41139,7 @@
       </c>
       <c r="AC26" s="6"/>
     </row>
-    <row r="27" spans="1:29" ht="16.2" thickBot="1">
+    <row r="27" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>25</v>
       </c>
@@ -41138,7 +41167,7 @@
       </c>
       <c r="AC27" s="8"/>
     </row>
-    <row r="28" spans="1:29" ht="16.2" thickBot="1">
+    <row r="28" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>26</v>
       </c>
@@ -41166,7 +41195,7 @@
       </c>
       <c r="AC28" s="6"/>
     </row>
-    <row r="29" spans="1:29" ht="16.2" thickBot="1">
+    <row r="29" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>27</v>
       </c>
@@ -41194,7 +41223,7 @@
       </c>
       <c r="AC29" s="8"/>
     </row>
-    <row r="30" spans="1:29" ht="16.2" thickBot="1">
+    <row r="30" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>28</v>
       </c>
@@ -41222,7 +41251,7 @@
       </c>
       <c r="AC30" s="6"/>
     </row>
-    <row r="31" spans="1:29" ht="16.2" thickBot="1">
+    <row r="31" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>29</v>
       </c>
@@ -41250,7 +41279,7 @@
       </c>
       <c r="AC31" s="6"/>
     </row>
-    <row r="32" spans="1:29" ht="16.2" thickBot="1">
+    <row r="32" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>30</v>
       </c>
@@ -41278,7 +41307,7 @@
       </c>
       <c r="AC32" s="8"/>
     </row>
-    <row r="33" spans="1:29" ht="16.2" thickBot="1">
+    <row r="33" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>31</v>
       </c>
@@ -41306,7 +41335,7 @@
       </c>
       <c r="AC33" s="6"/>
     </row>
-    <row r="34" spans="1:29" ht="16.2" thickBot="1">
+    <row r="34" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>32</v>
       </c>
@@ -41334,7 +41363,7 @@
       </c>
       <c r="AC34" s="6"/>
     </row>
-    <row r="35" spans="1:29" ht="16.2" thickBot="1">
+    <row r="35" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <v>33</v>
       </c>
@@ -41362,7 +41391,7 @@
       </c>
       <c r="AC35" s="8"/>
     </row>
-    <row r="36" spans="1:29" ht="16.2" thickBot="1">
+    <row r="36" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>34</v>
       </c>
@@ -41390,7 +41419,7 @@
       </c>
       <c r="AC36" s="6"/>
     </row>
-    <row r="37" spans="1:29" ht="16.2" thickBot="1">
+    <row r="37" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <v>35</v>
       </c>
@@ -41418,7 +41447,7 @@
       </c>
       <c r="AC37" s="6"/>
     </row>
-    <row r="38" spans="1:29" ht="16.2" thickBot="1">
+    <row r="38" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>36</v>
       </c>
@@ -41446,7 +41475,7 @@
       </c>
       <c r="AC38" s="8"/>
     </row>
-    <row r="39" spans="1:29" ht="16.2" thickBot="1">
+    <row r="39" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <v>37</v>
       </c>
@@ -41466,7 +41495,7 @@
       </c>
       <c r="AC39" s="6"/>
     </row>
-    <row r="40" spans="1:29" ht="16.2" thickBot="1">
+    <row r="40" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>38</v>
       </c>
@@ -41486,7 +41515,7 @@
       </c>
       <c r="AC40" s="6"/>
     </row>
-    <row r="41" spans="1:29" ht="16.2" thickBot="1">
+    <row r="41" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>39</v>
       </c>
@@ -41506,7 +41535,7 @@
       </c>
       <c r="AC41" s="8"/>
     </row>
-    <row r="42" spans="1:29" ht="16.2" thickBot="1">
+    <row r="42" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>40</v>
       </c>
@@ -41526,7 +41555,7 @@
       </c>
       <c r="AC42" s="6"/>
     </row>
-    <row r="43" spans="1:29" ht="16.2" thickBot="1">
+    <row r="43" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
         <v>41</v>
       </c>
@@ -41546,7 +41575,7 @@
       </c>
       <c r="AC43" s="6"/>
     </row>
-    <row r="44" spans="1:29" ht="16.2" thickBot="1">
+    <row r="44" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>42</v>
       </c>
@@ -41566,7 +41595,7 @@
       </c>
       <c r="AC44" s="8"/>
     </row>
-    <row r="45" spans="1:29" ht="16.2" thickBot="1">
+    <row r="45" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
         <v>43</v>
       </c>
@@ -41586,7 +41615,7 @@
       </c>
       <c r="AC45" s="6"/>
     </row>
-    <row r="46" spans="1:29" ht="16.2" thickBot="1">
+    <row r="46" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>44</v>
       </c>
@@ -41606,7 +41635,7 @@
       </c>
       <c r="AC46" s="6"/>
     </row>
-    <row r="47" spans="1:29" ht="16.2" thickBot="1">
+    <row r="47" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
         <v>45</v>
       </c>
@@ -41626,7 +41655,7 @@
       </c>
       <c r="AC47" s="8"/>
     </row>
-    <row r="48" spans="1:29" ht="16.2" thickBot="1">
+    <row r="48" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>46</v>
       </c>
@@ -41646,7 +41675,7 @@
       </c>
       <c r="AC48" s="6"/>
     </row>
-    <row r="49" spans="1:29" ht="16.2" thickBot="1">
+    <row r="49" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
         <v>47</v>
       </c>
@@ -41666,7 +41695,7 @@
       </c>
       <c r="AC49" s="6"/>
     </row>
-    <row r="50" spans="1:29" ht="16.2" thickBot="1">
+    <row r="50" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>48</v>
       </c>
@@ -41686,7 +41715,7 @@
       </c>
       <c r="AC50" s="8"/>
     </row>
-    <row r="51" spans="1:29" ht="16.2" thickBot="1">
+    <row r="51" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>49</v>
       </c>
@@ -41706,7 +41735,7 @@
       </c>
       <c r="AC51" s="6"/>
     </row>
-    <row r="52" spans="1:29" ht="16.2" thickBot="1">
+    <row r="52" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>50</v>
       </c>
@@ -41726,7 +41755,7 @@
       </c>
       <c r="AC52" s="6"/>
     </row>
-    <row r="53" spans="1:29" ht="16.2" thickBot="1">
+    <row r="53" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="7">
         <v>51</v>
       </c>
@@ -41746,7 +41775,7 @@
       </c>
       <c r="AC53" s="8"/>
     </row>
-    <row r="54" spans="1:29" ht="16.2" thickBot="1">
+    <row r="54" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>52</v>
       </c>
@@ -41766,7 +41795,7 @@
       </c>
       <c r="AC54" s="6"/>
     </row>
-    <row r="55" spans="1:29" ht="16.2" thickBot="1">
+    <row r="55" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="7">
         <v>53</v>
       </c>
@@ -41786,7 +41815,7 @@
       </c>
       <c r="AC55" s="6"/>
     </row>
-    <row r="56" spans="1:29" ht="16.2" thickBot="1">
+    <row r="56" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>54</v>
       </c>
@@ -41806,7 +41835,7 @@
       </c>
       <c r="AC56" s="8"/>
     </row>
-    <row r="57" spans="1:29" ht="16.2" thickBot="1">
+    <row r="57" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7">
         <v>55</v>
       </c>
@@ -41820,21 +41849,21 @@
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I57" s="18" t="s">
+      <c r="I57" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="J57" s="18"/>
-      <c r="K57" s="18"/>
-      <c r="L57" s="18"/>
-      <c r="M57" s="18"/>
-      <c r="N57" s="18"/>
+      <c r="J57" s="23"/>
+      <c r="K57" s="23"/>
+      <c r="L57" s="23"/>
+      <c r="M57" s="23"/>
+      <c r="N57" s="23"/>
       <c r="AB57" s="5" t="e">
         <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
       <c r="AC57" s="6"/>
     </row>
-    <row r="58" spans="1:29" ht="16.2" thickBot="1">
+    <row r="58" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>56</v>
       </c>
@@ -41848,16 +41877,16 @@
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I58" s="19"/>
-      <c r="J58" s="19"/>
-      <c r="K58" s="19"/>
-      <c r="L58" s="19"/>
-      <c r="M58" s="19"/>
-      <c r="N58" s="19"/>
+      <c r="I58" s="24"/>
+      <c r="J58" s="24"/>
+      <c r="K58" s="24"/>
+      <c r="L58" s="24"/>
+      <c r="M58" s="24"/>
+      <c r="N58" s="24"/>
       <c r="AB58" s="5"/>
       <c r="AC58" s="6"/>
     </row>
-    <row r="59" spans="1:29" ht="16.2" thickBot="1">
+    <row r="59" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7">
         <v>57</v>
       </c>
@@ -41874,7 +41903,7 @@
       <c r="AB59" s="5"/>
       <c r="AC59" s="8"/>
     </row>
-    <row r="60" spans="1:29" ht="16.2" thickBot="1">
+    <row r="60" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>58</v>
       </c>
@@ -41891,7 +41920,7 @@
       <c r="AB60" s="5"/>
       <c r="AC60" s="6"/>
     </row>
-    <row r="61" spans="1:29" ht="16.2" thickBot="1">
+    <row r="61" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7">
         <v>59</v>
       </c>
@@ -41908,7 +41937,7 @@
       <c r="AB61" s="5"/>
       <c r="AC61" s="6"/>
     </row>
-    <row r="62" spans="1:29" ht="16.2" thickBot="1">
+    <row r="62" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <v>60</v>
       </c>
@@ -41925,7 +41954,7 @@
       <c r="AB62" s="5"/>
       <c r="AC62" s="8"/>
     </row>
-    <row r="63" spans="1:29" ht="16.2" thickBot="1">
+    <row r="63" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="7">
         <v>61</v>
       </c>
@@ -41942,7 +41971,7 @@
       <c r="AB63" s="5"/>
       <c r="AC63" s="6"/>
     </row>
-    <row r="64" spans="1:29" ht="16.2" thickBot="1">
+    <row r="64" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
         <v>62</v>
       </c>
@@ -41957,7 +41986,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="16.2" thickBot="1">
+    <row r="65" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="7">
         <v>63</v>
       </c>
@@ -41972,7 +42001,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="16.2" thickBot="1">
+    <row r="66" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
         <v>64</v>
       </c>
@@ -41987,7 +42016,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="16.2" thickBot="1">
+    <row r="67" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A67" s="7">
         <v>65</v>
       </c>
@@ -42002,7 +42031,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="16.2" thickBot="1">
+    <row r="68" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
         <v>66</v>
       </c>
@@ -42017,7 +42046,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="16.2" thickBot="1">
+    <row r="69" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A69" s="7">
         <v>67</v>
       </c>
@@ -42032,7 +42061,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="16.2" thickBot="1">
+    <row r="70" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>68</v>
       </c>
@@ -42047,7 +42076,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="16.2" thickBot="1">
+    <row r="71" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A71" s="7">
         <v>69</v>
       </c>
@@ -42062,7 +42091,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="16.2" thickBot="1">
+    <row r="72" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
         <v>70</v>
       </c>
@@ -42077,7 +42106,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="16.2" thickBot="1">
+    <row r="73" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A73" s="7">
         <v>71</v>
       </c>
@@ -42092,7 +42121,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="16.2" thickBot="1">
+    <row r="74" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <v>72</v>
       </c>
@@ -42107,7 +42136,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="16.2" thickBot="1">
+    <row r="75" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A75" s="7">
         <v>73</v>
       </c>
@@ -42122,7 +42151,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="16.2" thickBot="1">
+    <row r="76" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A76" s="5">
         <v>74</v>
       </c>
@@ -42137,7 +42166,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="16.2" thickBot="1">
+    <row r="77" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A77" s="7">
         <v>75</v>
       </c>
@@ -42152,7 +42181,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="16.2" thickBot="1">
+    <row r="78" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
         <v>76</v>
       </c>
@@ -42167,7 +42196,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="16.2" thickBot="1">
+    <row r="79" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A79" s="7">
         <v>77</v>
       </c>
@@ -42182,7 +42211,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="16.2" thickBot="1">
+    <row r="80" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
         <v>78</v>
       </c>
@@ -42197,7 +42226,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="16.2" thickBot="1">
+    <row r="81" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A81" s="7">
         <v>79</v>
       </c>
@@ -42212,7 +42241,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="16.2" thickBot="1">
+    <row r="82" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A82" s="5">
         <v>80</v>
       </c>
@@ -42243,30 +42272,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86401310-AE3F-46D9-BA7D-9008211E0E75}">
   <dimension ref="A1:V8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="67" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P9" sqref="P7:P9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="11.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>35</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>36</v>
-      </c>
-      <c r="D1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" t="s">
-        <v>38</v>
       </c>
       <c r="G1" t="s">
         <v>26</v>
@@ -42275,7 +42305,10 @@
         <v>25</v>
       </c>
       <c r="J1" t="s">
-        <v>30</v>
+        <v>28</v>
+      </c>
+      <c r="K1" t="s">
+        <v>38</v>
       </c>
       <c r="M1" t="s">
         <v>24</v>
@@ -42284,28 +42317,28 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
-      <c r="A2">
-        <f>($P$4-$J$2)/$I$2</f>
-        <v>0.92049676874447606</v>
-      </c>
-      <c r="B2">
-        <f>($P$5-$J$2)/$I$2</f>
-        <v>0.93156594634823664</v>
-      </c>
-      <c r="C2">
-        <f>($P$5-$J$2)/$I$2</f>
-        <v>0.93156594634823664</v>
-      </c>
-      <c r="D2">
-        <f>($P$6-$J$2)/$I$2</f>
-        <v>0.94061012298368263</v>
-      </c>
-      <c r="E2">
-        <f>($P$7-$J$2)/$I$2</f>
-        <v>0.94825686537304998</v>
-      </c>
-      <c r="G2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2" s="21">
+        <f>LN($P$4/K2+1)/I2</f>
+        <v>0.57783361346788653</v>
+      </c>
+      <c r="B2" s="21">
+        <f>LN($P$5/K2+1)/I2</f>
+        <v>0.58890270444303594</v>
+      </c>
+      <c r="C2" s="21">
+        <f>LN($P$6/K2+1)/I2</f>
+        <v>0.59794682332599025</v>
+      </c>
+      <c r="D2" s="20">
+        <f>LN($P$7/K2+1)/I2</f>
+        <v>0.60559352446353687</v>
+      </c>
+      <c r="E2" s="20">
+        <f>LN($P$8/K2+1)/I2</f>
+        <v>0.61221740307494998</v>
+      </c>
+      <c r="G2" s="22">
         <f>60.5+273.15</f>
         <v>333.65</v>
       </c>
@@ -42315,35 +42348,39 @@
       <c r="J2">
         <v>-17.170000000000002</v>
       </c>
+      <c r="K2">
+        <f>EXP(J2)</f>
+        <v>3.4927197962393328E-8</v>
+      </c>
       <c r="M2">
         <v>1.702</v>
       </c>
       <c r="R2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
-      <c r="A3">
-        <f>($P$4-$J$3)/$I$3</f>
-        <v>0.91066617820949514</v>
-      </c>
-      <c r="B3">
-        <f>($P$6-$J$3)/$I$3</f>
-        <v>0.92871653248577901</v>
-      </c>
-      <c r="C3">
-        <f>($P$7-$J$3)/$I$3</f>
-        <v>0.93557895869008201</v>
-      </c>
-      <c r="D3">
-        <f>($P$8-$J$3)/$I$3</f>
-        <v>0.94152346265769638</v>
-      </c>
-      <c r="E3">
-        <f>($C$18-$J$3)/$I$3</f>
-        <v>0.84895160931309266</v>
-      </c>
-      <c r="G3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3" s="21">
+        <f t="shared" ref="A3:A6" si="0">LN($P$4/K3+1)/I3</f>
+        <v>0.60314919592841976</v>
+      </c>
+      <c r="B3" s="21">
+        <f t="shared" ref="B3:B7" si="1">LN($P$5/K3+1)/I3</f>
+        <v>0.61308301109620134</v>
+      </c>
+      <c r="C3" s="21">
+        <f t="shared" ref="C3:C7" si="2">LN($P$6/K3+1)/I3</f>
+        <v>0.62119953082465984</v>
+      </c>
+      <c r="D3" s="20">
+        <f t="shared" ref="D3:D7" si="3">LN($P$7/K3+1)/I3</f>
+        <v>0.62806195149180588</v>
+      </c>
+      <c r="E3" s="20">
+        <f t="shared" ref="E3:E7" si="4">LN($P$8/K3+1)/I3</f>
+        <v>0.6340064513065522</v>
+      </c>
+      <c r="G3" s="22">
         <f>47.7+273.15</f>
         <v>320.84999999999997</v>
       </c>
@@ -42353,47 +42390,48 @@
       <c r="J3">
         <v>-19.07</v>
       </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K7" si="5">EXP(J3)</f>
+        <v>5.2240127725508097E-9</v>
+      </c>
       <c r="M3">
         <v>1.6040000000000001</v>
       </c>
-      <c r="O3" t="s">
-        <v>28</v>
-      </c>
       <c r="P3" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="R3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="T3" t="s">
         <v>11</v>
       </c>
       <c r="V3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="17.399999999999999">
-      <c r="A4">
-        <f>($P$4-$J$4)/$I$4</f>
-        <v>0.92337789097613043</v>
-      </c>
-      <c r="B4">
-        <f>($P$5-$J$4)/$I$4</f>
-        <v>0.93299034687835358</v>
-      </c>
-      <c r="C4">
-        <f>($P$6-$J$4)/$I$4</f>
-        <v>0.94084429521961122</v>
-      </c>
-      <c r="D4">
-        <f>($P$7-$J$4)/$I$4</f>
-        <v>0.94748471392501565</v>
-      </c>
-      <c r="E4">
-        <f>($P$8-$J$4)/$I$4</f>
-        <v>0.95323690624966984</v>
-      </c>
-      <c r="G4">
+    <row r="4" spans="1:22" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="21">
+        <f>LN($P$4/K4+1)/I4</f>
+        <v>0.64480655629434747</v>
+      </c>
+      <c r="B4" s="21">
+        <f t="shared" si="1"/>
+        <v>0.65441900947683951</v>
+      </c>
+      <c r="C4" s="21">
+        <f t="shared" si="2"/>
+        <v>0.66227295600494307</v>
+      </c>
+      <c r="D4" s="20">
+        <f t="shared" si="3"/>
+        <v>0.66891337341523727</v>
+      </c>
+      <c r="E4" s="20">
+        <f>LN($P$8/K4+1)/I4</f>
+        <v>0.67466556476855888</v>
+      </c>
+      <c r="G4" s="22">
         <f>25.1+273.15</f>
         <v>298.25</v>
       </c>
@@ -42401,17 +42439,17 @@
         <v>23.213999999999999</v>
       </c>
       <c r="J4">
-        <v>-20.048999999999999</v>
+        <v>-20.49</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="5"/>
+        <v>1.262717111574683E-9</v>
       </c>
       <c r="M4">
         <v>1.6759999999999999</v>
       </c>
-      <c r="O4">
-        <v>4</v>
-      </c>
-      <c r="P4">
-        <f>LN(O4)</f>
-        <v>1.3862943611198906</v>
+      <c r="P4" s="18">
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="T4" s="9">
         <f>1.602176634*10^(-19)</f>
@@ -42422,28 +42460,28 @@
         <v>1.3806503000000004E-23</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
-      <c r="A5">
-        <f>($P$4-$J$5)/$I$5</f>
-        <v>0.94016288974212958</v>
-      </c>
-      <c r="B5">
-        <f>($P$5-$J$5)/$I$5</f>
-        <v>0.9490839928210969</v>
-      </c>
-      <c r="C5">
-        <f>($P$7-$J$5)/$I$5</f>
-        <v>0.96253588730081596</v>
-      </c>
-      <c r="D5">
-        <f>($P$4-$J$5)/$I$5</f>
-        <v>0.94016288974212958</v>
-      </c>
-      <c r="E5">
-        <f>($P$8-$J$5)/$I$5</f>
-        <v>0.96787436699635521</v>
-      </c>
-      <c r="G5">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A5" s="21">
+        <f t="shared" si="0"/>
+        <v>0.66399628766534324</v>
+      </c>
+      <c r="B5" s="21">
+        <f t="shared" si="1"/>
+        <v>0.67291739025468134</v>
+      </c>
+      <c r="C5" s="21">
+        <f t="shared" si="2"/>
+        <v>0.68020646188260381</v>
+      </c>
+      <c r="D5" s="20">
+        <f t="shared" si="3"/>
+        <v>0.68636928417482412</v>
+      </c>
+      <c r="E5" s="20">
+        <f>LN($P$8/K5+1)/I5</f>
+        <v>0.6917077636954958</v>
+      </c>
+      <c r="G5" s="22">
         <f>15.9+273.15</f>
         <v>289.04999999999995</v>
       </c>
@@ -42453,39 +42491,39 @@
       <c r="J5">
         <v>-22.13</v>
       </c>
+      <c r="K5">
+        <f t="shared" si="5"/>
+        <v>2.4494191870468971E-10</v>
+      </c>
       <c r="M5">
         <v>1.6040000000000001</v>
       </c>
-      <c r="O5">
-        <v>5</v>
-      </c>
-      <c r="P5">
-        <f>LN(O5)</f>
-        <v>1.6094379124341003</v>
+      <c r="P5" s="18">
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
-      <c r="A6">
-        <f>(P4-$J$6)/$I$6</f>
-        <v>0.96054622299964998</v>
-      </c>
-      <c r="B6">
-        <f>(P5-$J$6)/$I$6</f>
-        <v>0.96912108182892442</v>
-      </c>
-      <c r="C6">
-        <f>(P6-$J$6)/$I$6</f>
-        <v>0.97612725163232739</v>
-      </c>
-      <c r="D6">
-        <f>(P7-$J$6)/$I$6</f>
-        <v>0.98205088379722982</v>
-      </c>
-      <c r="E6">
-        <f>(P8-$J$6)/$I$6</f>
-        <v>0.98718216737808229</v>
-      </c>
-      <c r="G6">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A6" s="21">
+        <f t="shared" si="0"/>
+        <v>0.69509814764159616</v>
+      </c>
+      <c r="B6" s="21">
+        <f t="shared" si="1"/>
+        <v>0.70367300636373842</v>
+      </c>
+      <c r="C6" s="21">
+        <f t="shared" si="2"/>
+        <v>0.71067917609571996</v>
+      </c>
+      <c r="D6" s="20">
+        <f t="shared" si="3"/>
+        <v>0.7166028082096072</v>
+      </c>
+      <c r="E6" s="20">
+        <f t="shared" si="4"/>
+        <v>0.72173409175219805</v>
+      </c>
+      <c r="G6" s="22">
         <f>-0.6+273.15</f>
         <v>272.54999999999995</v>
       </c>
@@ -42495,39 +42533,39 @@
       <c r="J6">
         <v>-23.61</v>
       </c>
+      <c r="K6">
+        <f t="shared" si="5"/>
+        <v>5.5758012162231333E-11</v>
+      </c>
       <c r="M6">
         <v>1.637</v>
       </c>
-      <c r="O6">
-        <v>6</v>
-      </c>
-      <c r="P6">
-        <f>LN(O6)</f>
-        <v>1.791759469228055</v>
+      <c r="P6" s="18">
+        <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
-      <c r="A7">
-        <f>($P$4-$J$7)/$I$7</f>
-        <v>1.1277180816143892</v>
-      </c>
-      <c r="B7">
-        <f>($P5-$J$7)/$I$7</f>
-        <v>1.1303762929588912</v>
-      </c>
-      <c r="C7">
-        <f>($P$6-$J$7)/$I$7</f>
-        <v>1.1325482097710176</v>
-      </c>
-      <c r="D7">
-        <f>($P$7-$J$7)/$I$7</f>
-        <v>1.1343845392704188</v>
-      </c>
-      <c r="E7">
-        <f>($P$8-$J$7)/$I$7</f>
-        <v>1.1359752402368199</v>
-      </c>
-      <c r="G7">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A7" s="21">
+        <f>LN($P$4/K7+1)/I7</f>
+        <v>1.0454290199790073</v>
+      </c>
+      <c r="B7" s="21">
+        <f t="shared" si="1"/>
+        <v>1.0480872313235092</v>
+      </c>
+      <c r="C7" s="21">
+        <f t="shared" si="2"/>
+        <v>1.0502591481356356</v>
+      </c>
+      <c r="D7" s="20">
+        <f t="shared" si="3"/>
+        <v>1.0520954776350371</v>
+      </c>
+      <c r="E7" s="20">
+        <f t="shared" si="4"/>
+        <v>1.053686178601438</v>
+      </c>
+      <c r="G7" s="22">
         <v>77.2</v>
       </c>
       <c r="I7">
@@ -42536,25 +42574,313 @@
       <c r="J7">
         <v>-93.28</v>
       </c>
+      <c r="K7">
+        <f t="shared" si="5"/>
+        <v>3.0832641129675857E-41</v>
+      </c>
       <c r="M7">
         <v>1.7909999999999999</v>
       </c>
-      <c r="O7">
-        <v>7</v>
-      </c>
-      <c r="P7">
-        <f>LN(O7)</f>
-        <v>1.9459101490553132</v>
+      <c r="P7" s="18">
+        <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
-      <c r="O8">
-        <v>8</v>
-      </c>
-      <c r="P8">
-        <f>LN(O8)</f>
-        <v>2.0794415416798357</v>
-      </c>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="P8" s="18">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56093DD2-37EC-2948-87AD-2776D461F2EA}">
+  <dimension ref="A1:V9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2" s="21">
+        <f>LN($P$4/K2+1)/I2</f>
+        <v>0.57783361346788653</v>
+      </c>
+      <c r="B2" s="21">
+        <f>LN($P$5/K2+1)/I2</f>
+        <v>0.58890270444303594</v>
+      </c>
+      <c r="C2" s="21">
+        <f>LN($P$6/K2+1)/I2</f>
+        <v>0.59794682332599025</v>
+      </c>
+      <c r="D2" s="20">
+        <f>LN($P$7/K2+1)/I2</f>
+        <v>0.60559352446353687</v>
+      </c>
+      <c r="E2" s="20">
+        <f>LN($P$8/K2+1)/I2</f>
+        <v>0.61221740307494998</v>
+      </c>
+      <c r="G2" s="22">
+        <f>60.5+273.15</f>
+        <v>333.65</v>
+      </c>
+      <c r="I2">
+        <v>20.158999999999999</v>
+      </c>
+      <c r="J2">
+        <v>-17.170000000000002</v>
+      </c>
+      <c r="K2">
+        <f>EXP(J2)</f>
+        <v>3.4927197962393328E-8</v>
+      </c>
+      <c r="M2">
+        <v>1.702</v>
+      </c>
+      <c r="R2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3" s="21">
+        <f t="shared" ref="A3:A6" si="0">LN($P$4/K3+1)/I3</f>
+        <v>0.60314919592841976</v>
+      </c>
+      <c r="B3" s="21">
+        <f t="shared" ref="B3:B6" si="1">LN($P$5/K3+1)/I3</f>
+        <v>0.61308301109620134</v>
+      </c>
+      <c r="C3" s="21">
+        <f t="shared" ref="C3:C6" si="2">LN($P$6/K3+1)/I3</f>
+        <v>0.62119953082465984</v>
+      </c>
+      <c r="D3" s="20">
+        <f t="shared" ref="D3:D6" si="3">LN($P$7/K3+1)/I3</f>
+        <v>0.62806195149180588</v>
+      </c>
+      <c r="E3" s="20">
+        <f t="shared" ref="E3:E6" si="4">LN($P$8/K3+1)/I3</f>
+        <v>0.6340064513065522</v>
+      </c>
+      <c r="G3" s="22">
+        <f>47.7+273.15</f>
+        <v>320.84999999999997</v>
+      </c>
+      <c r="I3">
+        <v>22.463000000000001</v>
+      </c>
+      <c r="J3">
+        <v>-19.07</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K6" si="5">EXP(J3)</f>
+        <v>5.2240127725508097E-9</v>
+      </c>
+      <c r="M3">
+        <v>1.6040000000000001</v>
+      </c>
+      <c r="P3" t="s">
+        <v>37</v>
+      </c>
+      <c r="R3" t="s">
+        <v>30</v>
+      </c>
+      <c r="T3" t="s">
+        <v>11</v>
+      </c>
+      <c r="V3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="21">
+        <f>LN($P$4/K4+1)/I4</f>
+        <v>0.64480655629434747</v>
+      </c>
+      <c r="B4" s="21">
+        <f t="shared" si="1"/>
+        <v>0.65441900947683951</v>
+      </c>
+      <c r="C4" s="21">
+        <f t="shared" si="2"/>
+        <v>0.66227295600494307</v>
+      </c>
+      <c r="D4" s="20">
+        <f t="shared" si="3"/>
+        <v>0.66891337341523727</v>
+      </c>
+      <c r="E4" s="20">
+        <f>LN($P$8/K4+1)/I4</f>
+        <v>0.67466556476855888</v>
+      </c>
+      <c r="G4" s="22">
+        <f>25.1+273.15</f>
+        <v>298.25</v>
+      </c>
+      <c r="I4">
+        <v>23.213999999999999</v>
+      </c>
+      <c r="J4">
+        <v>-20.49</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="5"/>
+        <v>1.262717111574683E-9</v>
+      </c>
+      <c r="M4">
+        <v>1.6759999999999999</v>
+      </c>
+      <c r="P4" s="18">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="T4" s="9">
+        <f>1.602176634*10^(-19)</f>
+        <v>1.6021766340000001E-19</v>
+      </c>
+      <c r="V4" s="11">
+        <f>1.3806503*10^(-23)</f>
+        <v>1.3806503000000004E-23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A5" s="21">
+        <f t="shared" si="0"/>
+        <v>0.66399628766534324</v>
+      </c>
+      <c r="B5" s="21">
+        <f t="shared" si="1"/>
+        <v>0.67291739025468134</v>
+      </c>
+      <c r="C5" s="21">
+        <f t="shared" si="2"/>
+        <v>0.68020646188260381</v>
+      </c>
+      <c r="D5" s="20">
+        <f t="shared" si="3"/>
+        <v>0.68636928417482412</v>
+      </c>
+      <c r="E5" s="20">
+        <f>LN($P$8/K5+1)/I5</f>
+        <v>0.6917077636954958</v>
+      </c>
+      <c r="G5" s="22">
+        <f>15.9+273.15</f>
+        <v>289.04999999999995</v>
+      </c>
+      <c r="I5">
+        <v>25.013000000000002</v>
+      </c>
+      <c r="J5">
+        <v>-22.13</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="5"/>
+        <v>2.4494191870468971E-10</v>
+      </c>
+      <c r="M5">
+        <v>1.6040000000000001</v>
+      </c>
+      <c r="P5" s="18">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A6" s="21">
+        <f t="shared" si="0"/>
+        <v>0.69509814764159616</v>
+      </c>
+      <c r="B6" s="21">
+        <f t="shared" si="1"/>
+        <v>0.70367300636373842</v>
+      </c>
+      <c r="C6" s="21">
+        <f t="shared" si="2"/>
+        <v>0.71067917609571996</v>
+      </c>
+      <c r="D6" s="20">
+        <f t="shared" si="3"/>
+        <v>0.7166028082096072</v>
+      </c>
+      <c r="E6" s="20">
+        <f t="shared" si="4"/>
+        <v>0.72173409175219805</v>
+      </c>
+      <c r="G6" s="22">
+        <f>-0.6+273.15</f>
+        <v>272.54999999999995</v>
+      </c>
+      <c r="I6">
+        <v>26.023</v>
+      </c>
+      <c r="J6">
+        <v>-23.61</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="5"/>
+        <v>5.5758012162231333E-11</v>
+      </c>
+      <c r="M6">
+        <v>1.637</v>
+      </c>
+      <c r="P6" s="18">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="P7" s="18">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="P8" s="18">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="P9" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>